<commit_message>
通过 assetAllocationCategorySumParser 脚本的三级分类统计部分，成功更新 config/indexHoldingInfo.json
</commit_message>
<xml_diff>
--- a/Portfolio/scripts/output/201911/全家/全家整体收益估算.xlsx
+++ b/Portfolio/scripts/output/201911/全家/全家整体收益估算.xlsx
@@ -562,37 +562,37 @@
         <v>90010</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>1.6535</v>
+        <v>1.6525</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>2211.21</v>
+        <v>2280.92</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>3546.78</v>
+        <v>3667.72</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>-109.41</v>
+        <v>-101.61</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>1.61</v>
+        <v>1.608</v>
       </c>
       <c r="H2" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I2" s="4" t="n">
-        <v>1.6043</v>
+        <v>1.6048</v>
       </c>
       <c r="J2" s="7" t="n">
-        <v>-0.0035</v>
+        <v>-0.002</v>
       </c>
       <c r="K2" s="8" t="n">
-        <v>-12.6</v>
+        <v>-7.3</v>
       </c>
       <c r="L2" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M2" s="6" t="inlineStr">
@@ -631,37 +631,37 @@
         <v>519671</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>1.4258</v>
+        <v>1.4264</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>2462.53</v>
+        <v>2540.22</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>3499.26</v>
+        <v>3632.51</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>-11.88</v>
+        <v>9.130000000000001</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>1.425</v>
+        <v>1.43</v>
       </c>
       <c r="H3" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I3" s="4" t="n">
-        <v>1.4212</v>
+        <v>1.4235</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>-0.0027</v>
+        <v>-0.0046</v>
       </c>
       <c r="K3" s="8" t="n">
-        <v>-9.359999999999999</v>
+        <v>-16.51</v>
       </c>
       <c r="L3" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M3" s="6" t="inlineStr">
@@ -706,31 +706,31 @@
         <v>2260.14</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>3269.52</v>
+        <v>3301.61</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>222.58</v>
+        <v>254.67</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>1.4466</v>
+        <v>1.4608</v>
       </c>
       <c r="H4" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I4" s="4" t="n">
-        <v>1.4532</v>
+        <v>1.4338</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>0.0045</v>
-      </c>
-      <c r="K4" s="9" t="n">
-        <v>14.92</v>
+        <v>-0.0185</v>
+      </c>
+      <c r="K4" s="8" t="n">
+        <v>-61.02</v>
       </c>
       <c r="L4" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 16:00</t>
+          <t>2019-11-29 12:00</t>
         </is>
       </c>
       <c r="M4" s="6" t="inlineStr">
@@ -769,37 +769,37 @@
         <v>3318</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>0.9344</v>
+        <v>0.9336</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>3272.2</v>
+        <v>3390.61</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>2985.56</v>
+        <v>3082.4</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>-72</v>
+        <v>-83.01000000000001</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>0.9183</v>
+        <v>0.9091</v>
       </c>
       <c r="H5" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I5" s="4" t="n">
-        <v>0.9124</v>
+        <v>0.9094</v>
       </c>
       <c r="J5" s="7" t="n">
-        <v>-0.0065</v>
-      </c>
-      <c r="K5" s="8" t="n">
-        <v>-19.31</v>
+        <v>0.0004</v>
+      </c>
+      <c r="K5" s="9" t="n">
+        <v>1.02</v>
       </c>
       <c r="L5" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M5" s="6" t="inlineStr">
@@ -838,37 +838,37 @@
         <v>70023</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>1.7941</v>
+        <v>1.7965</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>1266.95</v>
+        <v>1314.93</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>2311.93</v>
+        <v>2419.47</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>38.85</v>
+        <v>57.15</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>1.8422</v>
+        <v>1.84</v>
       </c>
       <c r="H6" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I6" s="4" t="n">
-        <v>1.8247</v>
+        <v>1.8302</v>
       </c>
       <c r="J6" s="7" t="n">
-        <v>-0.0095</v>
+        <v>-0.0053</v>
       </c>
       <c r="K6" s="8" t="n">
-        <v>-22.17</v>
+        <v>-12.89</v>
       </c>
       <c r="L6" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M6" s="6" t="inlineStr">
@@ -907,37 +907,37 @@
         <v>530015</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>2.1197</v>
+        <v>2.1218</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>930.7</v>
+        <v>973.88</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>1973.83</v>
+        <v>2082.64</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.07</v>
+        <v>16.31</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>2.1379</v>
+        <v>2.1385</v>
       </c>
       <c r="H7" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I7" s="4" t="n">
-        <v>2.1202</v>
+        <v>2.1279</v>
       </c>
       <c r="J7" s="7" t="n">
-        <v>-0.0083</v>
+        <v>-0.0049</v>
       </c>
       <c r="K7" s="8" t="n">
-        <v>-16.47</v>
+        <v>-10.32</v>
       </c>
       <c r="L7" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M7" s="6" t="inlineStr">
@@ -976,37 +976,37 @@
         <v>968</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>0.9608</v>
+        <v>0.9605</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>797.84</v>
+        <v>887.74</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>762.58</v>
+        <v>840.6</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>-3.99</v>
+        <v>-12.08</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>0.9702</v>
+        <v>0.9469</v>
       </c>
       <c r="H8" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I8" s="4" t="n">
-        <v>0.9556</v>
+        <v>0.9376</v>
       </c>
       <c r="J8" s="7" t="n">
-        <v>-0.015</v>
+        <v>-0.0098</v>
       </c>
       <c r="K8" s="8" t="n">
-        <v>-11.65</v>
+        <v>-8.26</v>
       </c>
       <c r="L8" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M8" s="6" t="inlineStr">
@@ -1051,31 +1051,31 @@
         <v>550.4</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>512.48</v>
+        <v>513.3</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>-28.41</v>
+        <v>-27.59</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>0.9334</v>
+        <v>0.9326</v>
       </c>
       <c r="H9" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I9" s="4" t="n">
-        <v>0.9278</v>
+        <v>0.9268999999999999</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>-0.006</v>
+        <v>-0.0061</v>
       </c>
       <c r="K9" s="8" t="n">
-        <v>-3.08</v>
+        <v>-3.14</v>
       </c>
       <c r="L9" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M9" s="6" t="inlineStr">
@@ -1120,31 +1120,31 @@
         <v>531.87</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>415.39</v>
+        <v>410.5</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>58.61</v>
+        <v>53.72</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>0.8068</v>
+        <v>0.7718</v>
       </c>
       <c r="H10" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I10" s="4" t="n">
-        <v>0.7812</v>
+        <v>0.7577</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>-0.0317</v>
+        <v>-0.0182</v>
       </c>
       <c r="K10" s="8" t="n">
-        <v>-13.62</v>
+        <v>-7.5</v>
       </c>
       <c r="L10" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M10" s="6" t="inlineStr">
@@ -1189,31 +1189,31 @@
         <v>247.91</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>325.75</v>
+        <v>326.5</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>12.49</v>
+        <v>13.24</v>
       </c>
       <c r="G11" s="4" t="n">
-        <v>1.32</v>
+        <v>1.317</v>
       </c>
       <c r="H11" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I11" s="4" t="n">
-        <v>1.311</v>
+        <v>1.2915</v>
       </c>
       <c r="J11" s="7" t="n">
-        <v>-0.0068</v>
+        <v>-0.0194</v>
       </c>
       <c r="K11" s="8" t="n">
-        <v>-2.23</v>
+        <v>-6.32</v>
       </c>
       <c r="L11" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M11" s="6" t="inlineStr">
@@ -1258,31 +1258,31 @@
         <v>60.61</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>86.81</v>
+        <v>87.28</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>-5.9</v>
+        <v>-5.43</v>
       </c>
       <c r="G12" s="4" t="n">
-        <v>1.4361</v>
+        <v>1.44</v>
       </c>
       <c r="H12" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I12" s="4" t="n">
-        <v>1.4323</v>
+        <v>1.4334</v>
       </c>
       <c r="J12" s="7" t="n">
-        <v>-0.0027</v>
+        <v>-0.0046</v>
       </c>
       <c r="K12" s="8" t="n">
-        <v>-0.23</v>
+        <v>-0.4</v>
       </c>
       <c r="L12" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M12" s="6" t="inlineStr">
@@ -1327,31 +1327,31 @@
         <v>16731.88</v>
       </c>
       <c r="E13" s="13" t="n">
-        <v>9011.790000000001</v>
+        <v>9078.709999999999</v>
       </c>
       <c r="F13" s="13" t="n">
-        <v>-2988.21</v>
+        <v>-2921.28</v>
       </c>
       <c r="G13" s="12" t="n">
-        <v>0.5389</v>
+        <v>0.5426</v>
       </c>
       <c r="H13" s="14" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I13" s="12" t="n">
-        <v>0.5386</v>
+        <v>0.5413</v>
       </c>
       <c r="J13" s="15" t="n">
-        <v>-0.0005999999999999999</v>
+        <v>-0.0024</v>
       </c>
       <c r="K13" s="8" t="n">
-        <v>-5.02</v>
+        <v>-21.75</v>
       </c>
       <c r="L13" s="14" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M13" s="14" t="inlineStr">
@@ -1396,31 +1396,31 @@
         <v>2700</v>
       </c>
       <c r="E14" s="19" t="n">
-        <v>8010.9</v>
+        <v>8040.6</v>
       </c>
       <c r="F14" s="19" t="n">
-        <v>1701</v>
+        <v>1730.7</v>
       </c>
       <c r="G14" s="18" t="n">
-        <v>2.995</v>
+        <v>2.978</v>
       </c>
       <c r="H14" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I14" s="18" t="n">
-        <v>2.967</v>
+        <v>2.943</v>
       </c>
       <c r="J14" s="21" t="n">
-        <v>-0.009299999999999999</v>
+        <v>-0.0118</v>
       </c>
       <c r="K14" s="8" t="n">
-        <v>-75.59999999999999</v>
+        <v>-94.5</v>
       </c>
       <c r="L14" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:29</t>
         </is>
       </c>
       <c r="M14" s="20" t="inlineStr">
@@ -1465,31 +1465,31 @@
         <v>9100</v>
       </c>
       <c r="E15" s="19" t="n">
-        <v>35562.8</v>
+        <v>35763</v>
       </c>
       <c r="F15" s="19" t="n">
-        <v>4195.1</v>
+        <v>4395.3</v>
       </c>
       <c r="G15" s="18" t="n">
-        <v>3.95</v>
+        <v>3.93</v>
       </c>
       <c r="H15" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I15" s="18" t="n">
-        <v>3.908</v>
+        <v>3.886</v>
       </c>
       <c r="J15" s="21" t="n">
-        <v>-0.0106</v>
+        <v>-0.0112</v>
       </c>
       <c r="K15" s="8" t="n">
-        <v>-382.2</v>
+        <v>-400.4</v>
       </c>
       <c r="L15" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:29</t>
         </is>
       </c>
       <c r="M15" s="20" t="inlineStr">
@@ -1540,25 +1540,25 @@
         <v>-12066.8</v>
       </c>
       <c r="G16" s="18" t="n">
-        <v>5.345</v>
+        <v>5.29</v>
       </c>
       <c r="H16" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I16" s="18" t="n">
-        <v>5.29</v>
+        <v>5.279</v>
       </c>
       <c r="J16" s="21" t="n">
-        <v>-0.0103</v>
+        <v>-0.0021</v>
       </c>
       <c r="K16" s="8" t="n">
-        <v>-2134</v>
+        <v>-426.8</v>
       </c>
       <c r="L16" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:29</t>
         </is>
       </c>
       <c r="M16" s="20" t="inlineStr">
@@ -1603,21 +1603,21 @@
         <v>33800</v>
       </c>
       <c r="E17" s="19" t="n">
-        <v>24167</v>
+        <v>24403.6</v>
       </c>
       <c r="F17" s="19" t="n">
-        <v>-5475.6</v>
+        <v>-5239</v>
       </c>
       <c r="G17" s="18" t="n">
-        <v>0.716</v>
+        <v>0.722</v>
       </c>
       <c r="H17" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I17" s="18" t="n">
-        <v>0.715</v>
+        <v>0.721</v>
       </c>
       <c r="J17" s="21" t="n">
         <v>-0.0014</v>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="L17" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:26</t>
         </is>
       </c>
       <c r="M17" s="20" t="inlineStr">
@@ -1672,31 +1672,31 @@
         <v>32700</v>
       </c>
       <c r="E18" s="19" t="n">
-        <v>29397.3</v>
+        <v>29266.5</v>
       </c>
       <c r="F18" s="19" t="n">
-        <v>3793.2</v>
+        <v>3662.4</v>
       </c>
       <c r="G18" s="18" t="n">
-        <v>0.9</v>
+        <v>0.895</v>
       </c>
       <c r="H18" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I18" s="18" t="n">
         <v>0.899</v>
       </c>
       <c r="J18" s="21" t="n">
-        <v>-0.0011</v>
-      </c>
-      <c r="K18" s="8" t="n">
-        <v>-32.7</v>
+        <v>0.0045</v>
+      </c>
+      <c r="K18" s="9" t="n">
+        <v>130.8</v>
       </c>
       <c r="L18" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:29</t>
         </is>
       </c>
       <c r="M18" s="20" t="inlineStr">
@@ -1741,31 +1741,31 @@
         <v>34100</v>
       </c>
       <c r="E19" s="19" t="n">
-        <v>26052.4</v>
+        <v>25404.5</v>
       </c>
       <c r="F19" s="19" t="n">
-        <v>-3580.5</v>
+        <v>-4228.4</v>
       </c>
       <c r="G19" s="18" t="n">
-        <v>0.768</v>
+        <v>0.745</v>
       </c>
       <c r="H19" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I19" s="18" t="n">
-        <v>0.764</v>
+        <v>0.745</v>
       </c>
       <c r="J19" s="21" t="n">
-        <v>-0.0052</v>
-      </c>
-      <c r="K19" s="8" t="n">
-        <v>-136.4</v>
+        <v>0</v>
+      </c>
+      <c r="K19" s="9" t="n">
+        <v>0</v>
       </c>
       <c r="L19" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:29</t>
         </is>
       </c>
       <c r="M19" s="20" t="inlineStr">
@@ -1810,31 +1810,31 @@
         <v>4500</v>
       </c>
       <c r="E20" s="19" t="n">
-        <v>14791.5</v>
+        <v>14674.5</v>
       </c>
       <c r="F20" s="19" t="n">
-        <v>1939.5</v>
+        <v>1822.5</v>
       </c>
       <c r="G20" s="18" t="n">
-        <v>3.294</v>
+        <v>3.261</v>
       </c>
       <c r="H20" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I20" s="18" t="n">
-        <v>3.287</v>
+        <v>3.268</v>
       </c>
       <c r="J20" s="21" t="n">
-        <v>-0.0021</v>
-      </c>
-      <c r="K20" s="8" t="n">
-        <v>-31.5</v>
+        <v>0.0021</v>
+      </c>
+      <c r="K20" s="9" t="n">
+        <v>31.5</v>
       </c>
       <c r="L20" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:29</t>
         </is>
       </c>
       <c r="M20" s="20" t="inlineStr">
@@ -1879,31 +1879,31 @@
         <v>9200</v>
       </c>
       <c r="E21" s="19" t="n">
-        <v>14848.8</v>
+        <v>14821.2</v>
       </c>
       <c r="F21" s="19" t="n">
-        <v>1978</v>
+        <v>1950.4</v>
       </c>
       <c r="G21" s="18" t="n">
-        <v>1.65</v>
+        <v>1.611</v>
       </c>
       <c r="H21" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I21" s="18" t="n">
-        <v>1.614</v>
+        <v>1.596</v>
       </c>
       <c r="J21" s="21" t="n">
-        <v>-0.0218</v>
+        <v>-0.009299999999999999</v>
       </c>
       <c r="K21" s="8" t="n">
-        <v>-331.2</v>
+        <v>-138</v>
       </c>
       <c r="L21" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:04</t>
+          <t>2019-11-29 12:22</t>
         </is>
       </c>
       <c r="M21" s="20" t="inlineStr">
@@ -1948,31 +1948,31 @@
         <v>14400</v>
       </c>
       <c r="E22" s="19" t="n">
-        <v>19713.6</v>
+        <v>19569.6</v>
       </c>
       <c r="F22" s="19" t="n">
-        <v>1411.2</v>
+        <v>1267.2</v>
       </c>
       <c r="G22" s="18" t="n">
-        <v>1.414</v>
+        <v>1.359</v>
       </c>
       <c r="H22" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I22" s="18" t="n">
-        <v>1.369</v>
+        <v>1.326</v>
       </c>
       <c r="J22" s="21" t="n">
-        <v>-0.0318</v>
+        <v>-0.0243</v>
       </c>
       <c r="K22" s="8" t="n">
-        <v>-648</v>
+        <v>-475.2</v>
       </c>
       <c r="L22" s="20" t="inlineStr">
         <is>
-          <t>2019-11-22 15:04</t>
+          <t>2019-11-29 12:22</t>
         </is>
       </c>
       <c r="M22" s="20" t="inlineStr">
@@ -2017,31 +2017,31 @@
         <v>3813.64</v>
       </c>
       <c r="E23" s="25" t="n">
-        <v>7382.44</v>
+        <v>7368.33</v>
       </c>
       <c r="F23" s="25" t="n">
-        <v>45.44</v>
+        <v>31.33</v>
       </c>
       <c r="G23" s="24" t="n">
-        <v>1.9519</v>
+        <v>1.9321</v>
       </c>
       <c r="H23" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I23" s="24" t="n">
-        <v>1.9363</v>
+        <v>1.9271</v>
       </c>
       <c r="J23" s="27" t="n">
-        <v>-0.008</v>
+        <v>-0.0026</v>
       </c>
       <c r="K23" s="8" t="n">
-        <v>-59.49</v>
+        <v>-19.07</v>
       </c>
       <c r="L23" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M23" s="26" t="inlineStr">
@@ -2086,31 +2086,31 @@
         <v>9722</v>
       </c>
       <c r="E24" s="25" t="n">
-        <v>5236.27</v>
+        <v>5275.16</v>
       </c>
       <c r="F24" s="25" t="n">
-        <v>-99.73</v>
+        <v>-60.84</v>
       </c>
       <c r="G24" s="24" t="n">
-        <v>0.5389</v>
+        <v>0.5426</v>
       </c>
       <c r="H24" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I24" s="24" t="n">
-        <v>0.5386</v>
+        <v>0.5413</v>
       </c>
       <c r="J24" s="27" t="n">
-        <v>-0.0005999999999999999</v>
+        <v>-0.0024</v>
       </c>
       <c r="K24" s="8" t="n">
-        <v>-2.92</v>
+        <v>-12.64</v>
       </c>
       <c r="L24" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M24" s="26" t="inlineStr">
@@ -2155,31 +2155,31 @@
         <v>4943.96</v>
       </c>
       <c r="E25" s="25" t="n">
-        <v>4725.44</v>
+        <v>4681.44</v>
       </c>
       <c r="F25" s="25" t="n">
-        <v>56.44</v>
+        <v>12.44</v>
       </c>
       <c r="G25" s="24" t="n">
-        <v>0.9702</v>
+        <v>0.9469</v>
       </c>
       <c r="H25" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I25" s="24" t="n">
-        <v>0.9556</v>
+        <v>0.9376</v>
       </c>
       <c r="J25" s="27" t="n">
-        <v>-0.015</v>
+        <v>-0.0098</v>
       </c>
       <c r="K25" s="8" t="n">
-        <v>-72.18000000000001</v>
+        <v>-45.98</v>
       </c>
       <c r="L25" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M25" s="26" t="inlineStr">
@@ -2224,31 +2224,31 @@
         <v>7379.54</v>
       </c>
       <c r="E26" s="25" t="n">
-        <v>4021.85</v>
+        <v>4014.47</v>
       </c>
       <c r="F26" s="25" t="n">
-        <v>19.85</v>
+        <v>12.47</v>
       </c>
       <c r="G26" s="24" t="n">
-        <v>0.55</v>
+        <v>0.544</v>
       </c>
       <c r="H26" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I26" s="24" t="n">
-        <v>0.5456</v>
+        <v>0.5426</v>
       </c>
       <c r="J26" s="27" t="n">
-        <v>-0.008</v>
+        <v>-0.0026</v>
       </c>
       <c r="K26" s="8" t="n">
-        <v>-32.47</v>
+        <v>-10.33</v>
       </c>
       <c r="L26" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M26" s="26" t="inlineStr">
@@ -2293,31 +2293,31 @@
         <v>3665.01</v>
       </c>
       <c r="E27" s="25" t="n">
-        <v>3991.2</v>
+        <v>4002.19</v>
       </c>
       <c r="F27" s="25" t="n">
-        <v>-10.8</v>
+        <v>0.19</v>
       </c>
       <c r="G27" s="24" t="n">
-        <v>1.095</v>
+        <v>1.092</v>
       </c>
       <c r="H27" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I27" s="24" t="n">
-        <v>1.0912</v>
+        <v>1.0898</v>
       </c>
       <c r="J27" s="27" t="n">
-        <v>-0.0035</v>
+        <v>-0.002</v>
       </c>
       <c r="K27" s="8" t="n">
-        <v>-13.93</v>
+        <v>-8.06</v>
       </c>
       <c r="L27" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M27" s="26" t="inlineStr">
@@ -2362,31 +2362,31 @@
         <v>4550.55</v>
       </c>
       <c r="E28" s="25" t="n">
-        <v>3477.99</v>
+        <v>3405.18</v>
       </c>
       <c r="F28" s="25" t="n">
-        <v>142.99</v>
+        <v>70.18000000000001</v>
       </c>
       <c r="G28" s="24" t="n">
-        <v>0.772</v>
+        <v>0.7483</v>
       </c>
       <c r="H28" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I28" s="24" t="n">
-        <v>0.7643</v>
+        <v>0.7485000000000001</v>
       </c>
       <c r="J28" s="27" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="K28" s="8" t="n">
-        <v>-35.04</v>
+        <v>0.0003</v>
+      </c>
+      <c r="K28" s="9" t="n">
+        <v>0.91</v>
       </c>
       <c r="L28" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M28" s="26" t="inlineStr">
@@ -2431,31 +2431,31 @@
         <v>400.63</v>
       </c>
       <c r="E29" s="25" t="n">
-        <v>696.98</v>
+        <v>694.65</v>
       </c>
       <c r="F29" s="25" t="n">
-        <v>29.98</v>
+        <v>27.65</v>
       </c>
       <c r="G29" s="24" t="n">
-        <v>1.7723</v>
+        <v>1.7339</v>
       </c>
       <c r="H29" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I29" s="24" t="n">
-        <v>1.7395</v>
+        <v>1.7174</v>
       </c>
       <c r="J29" s="27" t="n">
-        <v>-0.0185</v>
+        <v>-0.0095</v>
       </c>
       <c r="K29" s="8" t="n">
-        <v>-13.14</v>
+        <v>-6.61</v>
       </c>
       <c r="L29" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M29" s="26" t="inlineStr">
@@ -2500,31 +2500,31 @@
         <v>736.3</v>
       </c>
       <c r="E30" s="25" t="n">
-        <v>696.25</v>
+        <v>693.37</v>
       </c>
       <c r="F30" s="25" t="n">
-        <v>29.25</v>
+        <v>26.37</v>
       </c>
       <c r="G30" s="24" t="n">
-        <v>0.9631</v>
+        <v>0.9417</v>
       </c>
       <c r="H30" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I30" s="24" t="n">
-        <v>0.9453</v>
+        <v>0.9328</v>
       </c>
       <c r="J30" s="27" t="n">
-        <v>-0.0185</v>
+        <v>-0.0095</v>
       </c>
       <c r="K30" s="8" t="n">
-        <v>-13.11</v>
+        <v>-6.55</v>
       </c>
       <c r="L30" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M30" s="26" t="inlineStr">
@@ -2569,31 +2569,31 @@
         <v>473.85</v>
       </c>
       <c r="E31" s="25" t="n">
-        <v>456.79</v>
+        <v>455.42</v>
       </c>
       <c r="F31" s="25" t="n">
-        <v>-10.11</v>
+        <v>-11.48</v>
       </c>
       <c r="G31" s="24" t="n">
-        <v>0.9671999999999999</v>
+        <v>0.9611</v>
       </c>
       <c r="H31" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I31" s="24" t="n">
-        <v>0.9643</v>
+        <v>0.965</v>
       </c>
       <c r="J31" s="27" t="n">
-        <v>-0.003</v>
-      </c>
-      <c r="K31" s="8" t="n">
-        <v>-1.37</v>
+        <v>0.0041</v>
+      </c>
+      <c r="K31" s="9" t="n">
+        <v>1.85</v>
       </c>
       <c r="L31" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M31" s="26" t="inlineStr">
@@ -2638,31 +2638,31 @@
         <v>5299.96</v>
       </c>
       <c r="E32" s="25" t="n">
-        <v>1982.18</v>
+        <v>1976.89</v>
       </c>
       <c r="F32" s="25" t="n">
-        <v>-18.81</v>
+        <v>-24.11</v>
       </c>
       <c r="G32" s="24" t="n">
-        <v>0.374</v>
+        <v>0.373</v>
       </c>
       <c r="H32" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="I32" s="24" t="n">
-        <v>0.3753</v>
+        <v>0.3735</v>
       </c>
       <c r="J32" s="27" t="n">
-        <v>0.0035</v>
+        <v>0.0014</v>
       </c>
       <c r="K32" s="9" t="n">
-        <v>6.89</v>
+        <v>2.65</v>
       </c>
       <c r="L32" s="26" t="inlineStr">
         <is>
-          <t>2019-11-23 05:00</t>
+          <t>2019-11-28 05:00</t>
         </is>
       </c>
       <c r="M32" s="26" t="inlineStr">
@@ -2707,31 +2707,31 @@
         <v>576.8</v>
       </c>
       <c r="E33" s="25" t="n">
-        <v>718.12</v>
+        <v>759.0700000000001</v>
       </c>
       <c r="F33" s="25" t="n">
-        <v>51.12</v>
+        <v>92.06999999999999</v>
       </c>
       <c r="G33" s="24" t="n">
-        <v>1.245</v>
+        <v>1.316</v>
       </c>
       <c r="H33" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="I33" s="24" t="n">
-        <v>1.2482</v>
+        <v>1.3174</v>
       </c>
       <c r="J33" s="27" t="n">
-        <v>0.0026</v>
+        <v>0.0011</v>
       </c>
       <c r="K33" s="9" t="n">
-        <v>1.85</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="L33" s="26" t="inlineStr">
         <is>
-          <t>2019-11-23 05:00</t>
+          <t>2019-11-28 05:00</t>
         </is>
       </c>
       <c r="M33" s="26" t="inlineStr">
@@ -2776,31 +2776,31 @@
         <v>459.67</v>
       </c>
       <c r="E34" s="25" t="n">
-        <v>685.46</v>
+        <v>691.76</v>
       </c>
       <c r="F34" s="25" t="n">
-        <v>18.46</v>
+        <v>24.76</v>
       </c>
       <c r="G34" s="24" t="n">
-        <v>1.4912</v>
+        <v>1.5049</v>
       </c>
       <c r="H34" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I34" s="24" t="n">
-        <v>1.4981</v>
+        <v>1.4767</v>
       </c>
       <c r="J34" s="27" t="n">
-        <v>0.0046</v>
-      </c>
-      <c r="K34" s="9" t="n">
-        <v>3.17</v>
+        <v>-0.0187</v>
+      </c>
+      <c r="K34" s="8" t="n">
+        <v>-12.96</v>
       </c>
       <c r="L34" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 16:00</t>
+          <t>2019-11-29 12:00</t>
         </is>
       </c>
       <c r="M34" s="26" t="inlineStr">
@@ -2845,10 +2845,10 @@
         <v>611.75</v>
       </c>
       <c r="E35" s="25" t="n">
-        <v>734.71</v>
+        <v>739.61</v>
       </c>
       <c r="F35" s="25" t="n">
-        <v>67.70999999999999</v>
+        <v>72.61</v>
       </c>
       <c r="G35" s="24" t="n">
         <v>0</v>
@@ -2914,31 +2914,31 @@
         <v>1046.73</v>
       </c>
       <c r="E36" s="25" t="n">
-        <v>2026.26</v>
+        <v>2022.39</v>
       </c>
       <c r="F36" s="25" t="n">
-        <v>26.26</v>
+        <v>22.39</v>
       </c>
       <c r="G36" s="24" t="n">
-        <v>1.9519</v>
+        <v>1.9321</v>
       </c>
       <c r="H36" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I36" s="24" t="n">
-        <v>1.9363</v>
+        <v>1.9271</v>
       </c>
       <c r="J36" s="27" t="n">
-        <v>-0.008</v>
+        <v>-0.0026</v>
       </c>
       <c r="K36" s="8" t="n">
-        <v>-16.33</v>
+        <v>-5.23</v>
       </c>
       <c r="L36" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M36" s="26" t="inlineStr">
@@ -2983,31 +2983,31 @@
         <v>1825.9</v>
       </c>
       <c r="E37" s="25" t="n">
-        <v>1988.41</v>
+        <v>1993.88</v>
       </c>
       <c r="F37" s="25" t="n">
-        <v>-11.59</v>
+        <v>-6.12</v>
       </c>
       <c r="G37" s="24" t="n">
-        <v>1.095</v>
+        <v>1.092</v>
       </c>
       <c r="H37" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I37" s="24" t="n">
-        <v>1.0912</v>
+        <v>1.0898</v>
       </c>
       <c r="J37" s="27" t="n">
-        <v>-0.0035</v>
+        <v>-0.002</v>
       </c>
       <c r="K37" s="8" t="n">
-        <v>-6.94</v>
+        <v>-4.02</v>
       </c>
       <c r="L37" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M37" s="26" t="inlineStr">
@@ -3052,31 +3052,31 @@
         <v>1059.17</v>
       </c>
       <c r="E38" s="25" t="n">
-        <v>1060.23</v>
+        <v>1063.41</v>
       </c>
       <c r="F38" s="25" t="n">
-        <v>60.23</v>
+        <v>63.41</v>
       </c>
       <c r="G38" s="24" t="n">
-        <v>1.01</v>
+        <v>1.004</v>
       </c>
       <c r="H38" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I38" s="24" t="n">
-        <v>1.0012</v>
+        <v>0.9925</v>
       </c>
       <c r="J38" s="27" t="n">
-        <v>-0.008699999999999999</v>
+        <v>-0.0115</v>
       </c>
       <c r="K38" s="8" t="n">
-        <v>-9.32</v>
+        <v>-12.18</v>
       </c>
       <c r="L38" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M38" s="26" t="inlineStr">
@@ -3121,31 +3121,31 @@
         <v>1812.7</v>
       </c>
       <c r="E39" s="25" t="n">
-        <v>987.92</v>
+        <v>986.11</v>
       </c>
       <c r="F39" s="25" t="n">
-        <v>-12.08</v>
+        <v>-13.89</v>
       </c>
       <c r="G39" s="24" t="n">
-        <v>0.55</v>
+        <v>0.544</v>
       </c>
       <c r="H39" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I39" s="24" t="n">
-        <v>0.5456</v>
+        <v>0.5426</v>
       </c>
       <c r="J39" s="27" t="n">
-        <v>-0.008</v>
+        <v>-0.0026</v>
       </c>
       <c r="K39" s="8" t="n">
-        <v>-7.98</v>
+        <v>-2.54</v>
       </c>
       <c r="L39" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M39" s="26" t="inlineStr">
@@ -3190,31 +3190,31 @@
         <v>1227.03</v>
       </c>
       <c r="E40" s="25" t="n">
-        <v>937.8200000000001</v>
+        <v>918.1900000000001</v>
       </c>
       <c r="F40" s="25" t="n">
-        <v>-62.18</v>
+        <v>-81.81</v>
       </c>
       <c r="G40" s="24" t="n">
-        <v>0.772</v>
+        <v>0.7483</v>
       </c>
       <c r="H40" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I40" s="24" t="n">
-        <v>0.7643</v>
+        <v>0.7485000000000001</v>
       </c>
       <c r="J40" s="27" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="K40" s="8" t="n">
-        <v>-9.449999999999999</v>
+        <v>0.0003</v>
+      </c>
+      <c r="K40" s="9" t="n">
+        <v>0.25</v>
       </c>
       <c r="L40" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M40" s="26" t="inlineStr">
@@ -3246,64 +3246,64 @@
     <row r="41">
       <c r="A41" s="22" t="inlineStr">
         <is>
-          <t>华安黄金易ETF联接A</t>
+          <t>交银中证海外中国互联网指数</t>
         </is>
       </c>
       <c r="B41" s="23" t="n">
-        <v>216</v>
+        <v>164906</v>
       </c>
       <c r="C41" s="24" t="n">
-        <v>1.0902</v>
+        <v>1.1113</v>
       </c>
       <c r="D41" s="25" t="n">
-        <v>1834.47</v>
+        <v>899.8200000000001</v>
       </c>
       <c r="E41" s="25" t="n">
-        <v>2240.44</v>
+        <v>1184.16</v>
       </c>
       <c r="F41" s="25" t="n">
-        <v>240.44</v>
+        <v>184.16</v>
       </c>
       <c r="G41" s="24" t="n">
-        <v>1.2202</v>
+        <v>1.316</v>
       </c>
       <c r="H41" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="I41" s="24" t="n">
-        <v>1.2219</v>
+        <v>1.3174</v>
       </c>
       <c r="J41" s="27" t="n">
-        <v>0.0014</v>
+        <v>0.0011</v>
       </c>
       <c r="K41" s="9" t="n">
-        <v>3.12</v>
+        <v>1.26</v>
       </c>
       <c r="L41" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 15:30</t>
+          <t>2019-11-28 05:00</t>
         </is>
       </c>
       <c r="M41" s="26" t="inlineStr">
         <is>
-          <t>商品</t>
+          <t>海外新兴</t>
         </is>
       </c>
       <c r="N41" s="26" t="inlineStr">
         <is>
-          <t>商品</t>
+          <t>海外互联</t>
         </is>
       </c>
       <c r="O41" s="26" t="inlineStr">
         <is>
-          <t>黄金</t>
+          <t>海外互联网</t>
         </is>
       </c>
       <c r="P41" s="26" t="inlineStr">
         <is>
-          <t>511</t>
+          <t>213</t>
         </is>
       </c>
       <c r="Q41" s="26" t="inlineStr">
@@ -3315,44 +3315,44 @@
     <row r="42">
       <c r="A42" s="22" t="inlineStr">
         <is>
-          <t>交银中证海外中国互联网指数</t>
+          <t>华夏恒生ETF联接A</t>
         </is>
       </c>
       <c r="B42" s="23" t="n">
-        <v>164906</v>
+        <v>71</v>
       </c>
       <c r="C42" s="24" t="n">
-        <v>1.1113</v>
+        <v>1.4513</v>
       </c>
       <c r="D42" s="25" t="n">
-        <v>899.8200000000001</v>
+        <v>689.02</v>
       </c>
       <c r="E42" s="25" t="n">
-        <v>1120.28</v>
+        <v>1036.91</v>
       </c>
       <c r="F42" s="25" t="n">
-        <v>120.28</v>
+        <v>36.91</v>
       </c>
       <c r="G42" s="24" t="n">
-        <v>1.245</v>
+        <v>1.5049</v>
       </c>
       <c r="H42" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I42" s="24" t="n">
-        <v>1.2482</v>
+        <v>1.4767</v>
       </c>
       <c r="J42" s="27" t="n">
-        <v>0.0026</v>
-      </c>
-      <c r="K42" s="9" t="n">
-        <v>2.88</v>
+        <v>-0.0187</v>
+      </c>
+      <c r="K42" s="8" t="n">
+        <v>-19.43</v>
       </c>
       <c r="L42" s="26" t="inlineStr">
         <is>
-          <t>2019-11-23 05:00</t>
+          <t>2019-11-29 12:00</t>
         </is>
       </c>
       <c r="M42" s="26" t="inlineStr">
@@ -3362,17 +3362,17 @@
       </c>
       <c r="N42" s="26" t="inlineStr">
         <is>
-          <t>海外互联</t>
+          <t>香港</t>
         </is>
       </c>
       <c r="O42" s="26" t="inlineStr">
         <is>
-          <t>海外互联网</t>
+          <t>恒生</t>
         </is>
       </c>
       <c r="P42" s="26" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>211</t>
         </is>
       </c>
       <c r="Q42" s="26" t="inlineStr">
@@ -3384,64 +3384,64 @@
     <row r="43">
       <c r="A43" s="22" t="inlineStr">
         <is>
-          <t>华夏恒生ETF联接A</t>
+          <t>华安黄金易ETF联接A</t>
         </is>
       </c>
       <c r="B43" s="23" t="n">
-        <v>71</v>
+        <v>216</v>
       </c>
       <c r="C43" s="24" t="n">
-        <v>1.4513</v>
+        <v>1.0902</v>
       </c>
       <c r="D43" s="25" t="n">
-        <v>689.02</v>
+        <v>1834.47</v>
       </c>
       <c r="E43" s="25" t="n">
-        <v>1027.47</v>
+        <v>2218.42</v>
       </c>
       <c r="F43" s="25" t="n">
-        <v>27.47</v>
+        <v>218.42</v>
       </c>
       <c r="G43" s="24" t="n">
-        <v>1.4912</v>
+        <v>1.2093</v>
       </c>
       <c r="H43" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I43" s="24" t="n">
-        <v>1.4981</v>
+        <v>1.2098</v>
       </c>
       <c r="J43" s="27" t="n">
-        <v>0.0046</v>
+        <v>0.0005</v>
       </c>
       <c r="K43" s="9" t="n">
-        <v>4.75</v>
+        <v>0.92</v>
       </c>
       <c r="L43" s="26" t="inlineStr">
         <is>
-          <t>2019-11-22 16:00</t>
+          <t>2019-11-29 11:35</t>
         </is>
       </c>
       <c r="M43" s="26" t="inlineStr">
         <is>
-          <t>海外新兴</t>
+          <t>商品</t>
         </is>
       </c>
       <c r="N43" s="26" t="inlineStr">
         <is>
-          <t>香港</t>
+          <t>商品</t>
         </is>
       </c>
       <c r="O43" s="26" t="inlineStr">
         <is>
-          <t>恒生</t>
+          <t>黄金</t>
         </is>
       </c>
       <c r="P43" s="26" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>511</t>
         </is>
       </c>
       <c r="Q43" s="26" t="inlineStr">
@@ -3466,31 +3466,31 @@
         <v>4757.9</v>
       </c>
       <c r="E44" s="25" t="n">
-        <v>1779.45</v>
+        <v>1774.7</v>
       </c>
       <c r="F44" s="25" t="n">
-        <v>-220.55</v>
+        <v>-225.3</v>
       </c>
       <c r="G44" s="24" t="n">
-        <v>0.374</v>
+        <v>0.373</v>
       </c>
       <c r="H44" s="26" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="I44" s="24" t="n">
-        <v>0.3753</v>
+        <v>0.3735</v>
       </c>
       <c r="J44" s="27" t="n">
-        <v>0.0035</v>
+        <v>0.0014</v>
       </c>
       <c r="K44" s="9" t="n">
-        <v>6.19</v>
+        <v>2.38</v>
       </c>
       <c r="L44" s="26" t="inlineStr">
         <is>
-          <t>2019-11-23 05:00</t>
+          <t>2019-11-28 05:00</t>
         </is>
       </c>
       <c r="M44" s="26" t="inlineStr">
@@ -3535,10 +3535,10 @@
         <v>953.96</v>
       </c>
       <c r="E45" s="25" t="n">
-        <v>1145.71</v>
+        <v>1153.34</v>
       </c>
       <c r="F45" s="25" t="n">
-        <v>145.71</v>
+        <v>153.34</v>
       </c>
       <c r="G45" s="24" t="n">
         <v>0</v>
@@ -3604,31 +3604,31 @@
         <v>65064.33</v>
       </c>
       <c r="E46" s="31" t="n">
-        <v>70855.05</v>
+        <v>71050.24000000001</v>
       </c>
       <c r="F46" s="31" t="n">
-        <v>4535.05</v>
+        <v>4730.24</v>
       </c>
       <c r="G46" s="30" t="n">
-        <v>1.095</v>
+        <v>1.092</v>
       </c>
       <c r="H46" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I46" s="30" t="n">
-        <v>1.0912</v>
+        <v>1.0898</v>
       </c>
       <c r="J46" s="33" t="n">
-        <v>-0.0035</v>
+        <v>-0.002</v>
       </c>
       <c r="K46" s="8" t="n">
-        <v>-247.24</v>
+        <v>-143.14</v>
       </c>
       <c r="L46" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M46" s="32" t="inlineStr">
@@ -3673,31 +3673,31 @@
         <v>63490</v>
       </c>
       <c r="E47" s="31" t="n">
-        <v>60683.74</v>
+        <v>60118.68</v>
       </c>
       <c r="F47" s="31" t="n">
-        <v>2483.74</v>
+        <v>1918.68</v>
       </c>
       <c r="G47" s="30" t="n">
-        <v>0.9702</v>
+        <v>0.9469</v>
       </c>
       <c r="H47" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I47" s="30" t="n">
-        <v>0.9556</v>
+        <v>0.9376</v>
       </c>
       <c r="J47" s="33" t="n">
-        <v>-0.015</v>
+        <v>-0.0098</v>
       </c>
       <c r="K47" s="8" t="n">
-        <v>-926.95</v>
+        <v>-590.46</v>
       </c>
       <c r="L47" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M47" s="32" t="inlineStr">
@@ -3742,31 +3742,31 @@
         <v>32370.29</v>
       </c>
       <c r="E48" s="31" t="n">
-        <v>37054.27</v>
+        <v>37080.16</v>
       </c>
       <c r="F48" s="31" t="n">
-        <v>5054.27</v>
+        <v>5080.16</v>
       </c>
       <c r="G48" s="30" t="n">
-        <v>1.1484</v>
+        <v>1.1455</v>
       </c>
       <c r="H48" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I48" s="30" t="n">
-        <v>1.1459</v>
+        <v>1.1442</v>
       </c>
       <c r="J48" s="33" t="n">
-        <v>-0.0022</v>
+        <v>-0.0012</v>
       </c>
       <c r="K48" s="8" t="n">
-        <v>-80.93000000000001</v>
+        <v>-42.08</v>
       </c>
       <c r="L48" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M48" s="32" t="inlineStr">
@@ -3811,31 +3811,31 @@
         <v>41014.88</v>
       </c>
       <c r="E49" s="31" t="n">
-        <v>35051.31</v>
+        <v>34760.11</v>
       </c>
       <c r="F49" s="31" t="n">
-        <v>4491.31</v>
+        <v>4200.11</v>
       </c>
       <c r="G49" s="30" t="n">
-        <v>0.8803</v>
+        <v>0.8475</v>
       </c>
       <c r="H49" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I49" s="30" t="n">
-        <v>0.8542999999999999</v>
+        <v>0.8276</v>
       </c>
       <c r="J49" s="33" t="n">
-        <v>-0.0295</v>
+        <v>-0.0235</v>
       </c>
       <c r="K49" s="8" t="n">
-        <v>-1066.39</v>
+        <v>-816.2</v>
       </c>
       <c r="L49" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M49" s="32" t="inlineStr">
@@ -3886,25 +3886,25 @@
         <v>1765.62</v>
       </c>
       <c r="G50" s="30" t="n">
-        <v>1.688</v>
+        <v>1.681</v>
       </c>
       <c r="H50" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I50" s="30" t="n">
-        <v>1.6841</v>
+        <v>1.678</v>
       </c>
       <c r="J50" s="33" t="n">
-        <v>-0.0023</v>
+        <v>-0.0018</v>
       </c>
       <c r="K50" s="8" t="n">
-        <v>-78.34</v>
+        <v>-60.26</v>
       </c>
       <c r="L50" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M50" s="32" t="inlineStr">
@@ -3949,10 +3949,10 @@
         <v>20716.63</v>
       </c>
       <c r="E51" s="31" t="n">
-        <v>24880.67</v>
+        <v>25046.4</v>
       </c>
       <c r="F51" s="31" t="n">
-        <v>2280.67</v>
+        <v>2446.4</v>
       </c>
       <c r="G51" s="30" t="n">
         <v>0</v>
@@ -4018,31 +4018,31 @@
         <v>14624.61</v>
       </c>
       <c r="E52" s="31" t="n">
-        <v>23501.74</v>
+        <v>23530.99</v>
       </c>
       <c r="F52" s="31" t="n">
-        <v>4301.74</v>
+        <v>4330.99</v>
       </c>
       <c r="G52" s="30" t="n">
-        <v>1.626</v>
+        <v>1.609</v>
       </c>
       <c r="H52" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I52" s="30" t="n">
-        <v>1.6102</v>
+        <v>1.5936</v>
       </c>
       <c r="J52" s="33" t="n">
-        <v>-0.0097</v>
+        <v>-0.009599999999999999</v>
       </c>
       <c r="K52" s="8" t="n">
-        <v>-231.07</v>
+        <v>-225.22</v>
       </c>
       <c r="L52" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M52" s="32" t="inlineStr">
@@ -4087,31 +4087,31 @@
         <v>21163.93</v>
       </c>
       <c r="E53" s="31" t="n">
-        <v>22810.48</v>
+        <v>22840.11</v>
       </c>
       <c r="F53" s="31" t="n">
-        <v>3610.48</v>
+        <v>3640.11</v>
       </c>
       <c r="G53" s="30" t="n">
-        <v>1.0826</v>
+        <v>1.0792</v>
       </c>
       <c r="H53" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I53" s="30" t="n">
-        <v>1.0777</v>
+        <v>1.0764</v>
       </c>
       <c r="J53" s="33" t="n">
-        <v>-0.0046</v>
+        <v>-0.0026</v>
       </c>
       <c r="K53" s="8" t="n">
-        <v>-103.7</v>
+        <v>-59.26</v>
       </c>
       <c r="L53" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M53" s="32" t="inlineStr">
@@ -4156,31 +4156,31 @@
         <v>16778.47</v>
       </c>
       <c r="E54" s="31" t="n">
-        <v>20889.19</v>
+        <v>22080.46</v>
       </c>
       <c r="F54" s="31" t="n">
-        <v>1689.19</v>
+        <v>2880.46</v>
       </c>
       <c r="G54" s="30" t="n">
-        <v>1.245</v>
+        <v>1.316</v>
       </c>
       <c r="H54" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="I54" s="30" t="n">
-        <v>1.2482</v>
+        <v>1.3174</v>
       </c>
       <c r="J54" s="33" t="n">
-        <v>0.0026</v>
+        <v>0.0011</v>
       </c>
       <c r="K54" s="9" t="n">
-        <v>53.69</v>
+        <v>23.49</v>
       </c>
       <c r="L54" s="32" t="inlineStr">
         <is>
-          <t>2019-11-23 05:00</t>
+          <t>2019-11-28 05:00</t>
         </is>
       </c>
       <c r="M54" s="32" t="inlineStr">
@@ -4225,31 +4225,31 @@
         <v>9529.809999999999</v>
       </c>
       <c r="E55" s="31" t="n">
-        <v>15133.33</v>
+        <v>15114.27</v>
       </c>
       <c r="F55" s="31" t="n">
-        <v>2333.33</v>
+        <v>2314.27</v>
       </c>
       <c r="G55" s="30" t="n">
-        <v>1.605</v>
+        <v>1.586</v>
       </c>
       <c r="H55" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I55" s="30" t="n">
-        <v>1.5922</v>
+        <v>1.5819</v>
       </c>
       <c r="J55" s="33" t="n">
-        <v>-0.008</v>
+        <v>-0.0026</v>
       </c>
       <c r="K55" s="8" t="n">
-        <v>-121.98</v>
+        <v>-39.07</v>
       </c>
       <c r="L55" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M55" s="32" t="inlineStr">
@@ -4294,31 +4294,31 @@
         <v>37267.45</v>
       </c>
       <c r="E56" s="31" t="n">
-        <v>13938.02</v>
+        <v>13900.75</v>
       </c>
       <c r="F56" s="31" t="n">
-        <v>-5261.98</v>
+        <v>-5299.25</v>
       </c>
       <c r="G56" s="30" t="n">
-        <v>0.374</v>
+        <v>0.373</v>
       </c>
       <c r="H56" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="I56" s="30" t="n">
-        <v>0.3753</v>
+        <v>0.3735</v>
       </c>
       <c r="J56" s="33" t="n">
-        <v>0.0035</v>
+        <v>0.0014</v>
       </c>
       <c r="K56" s="9" t="n">
-        <v>48.45</v>
+        <v>18.63</v>
       </c>
       <c r="L56" s="32" t="inlineStr">
         <is>
-          <t>2019-11-23 05:00</t>
+          <t>2019-11-28 05:00</t>
         </is>
       </c>
       <c r="M56" s="32" t="inlineStr">
@@ -4363,31 +4363,31 @@
         <v>6798.52</v>
       </c>
       <c r="E57" s="31" t="n">
-        <v>10137.95</v>
+        <v>10231.09</v>
       </c>
       <c r="F57" s="31" t="n">
-        <v>237.95</v>
+        <v>331.09</v>
       </c>
       <c r="G57" s="30" t="n">
-        <v>1.4912</v>
+        <v>1.5049</v>
       </c>
       <c r="H57" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I57" s="30" t="n">
-        <v>1.4981</v>
+        <v>1.4767</v>
       </c>
       <c r="J57" s="33" t="n">
-        <v>0.0046</v>
-      </c>
-      <c r="K57" s="9" t="n">
-        <v>46.91</v>
+        <v>-0.0187</v>
+      </c>
+      <c r="K57" s="8" t="n">
+        <v>-191.72</v>
       </c>
       <c r="L57" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 16:00</t>
+          <t>2019-11-29 12:00</t>
         </is>
       </c>
       <c r="M57" s="32" t="inlineStr">
@@ -4432,31 +4432,31 @@
         <v>4791.13</v>
       </c>
       <c r="E58" s="31" t="n">
-        <v>8335.120000000001</v>
+        <v>8307.34</v>
       </c>
       <c r="F58" s="31" t="n">
-        <v>1935.12</v>
+        <v>1907.34</v>
       </c>
       <c r="G58" s="30" t="n">
-        <v>1.7723</v>
+        <v>1.7339</v>
       </c>
       <c r="H58" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I58" s="30" t="n">
-        <v>1.7395</v>
+        <v>1.7174</v>
       </c>
       <c r="J58" s="33" t="n">
-        <v>-0.0185</v>
+        <v>-0.0095</v>
       </c>
       <c r="K58" s="8" t="n">
-        <v>-157.15</v>
+        <v>-79.05</v>
       </c>
       <c r="L58" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M58" s="32" t="inlineStr">
@@ -4501,10 +4501,10 @@
         <v>5609.79</v>
       </c>
       <c r="E59" s="31" t="n">
-        <v>7533.94</v>
+        <v>7567.6</v>
       </c>
       <c r="F59" s="31" t="n">
-        <v>2388.82</v>
+        <v>2422.48</v>
       </c>
       <c r="G59" s="30" t="n">
         <v>0</v>
@@ -4557,64 +4557,64 @@
     <row r="60">
       <c r="A60" s="28" t="inlineStr">
         <is>
-          <t>长信可转债债券A</t>
+          <t>广发中证环保ETF联接A</t>
         </is>
       </c>
       <c r="B60" s="29" t="n">
-        <v>519977</v>
+        <v>1064</v>
       </c>
       <c r="C60" s="30" t="n">
-        <v>1.2011</v>
+        <v>0.4775</v>
       </c>
       <c r="D60" s="31" t="n">
-        <v>5328.62</v>
+        <v>13403.92</v>
       </c>
       <c r="E60" s="31" t="n">
-        <v>7232</v>
+        <v>7272.96</v>
       </c>
       <c r="F60" s="31" t="n">
-        <v>832</v>
+        <v>872.96</v>
       </c>
       <c r="G60" s="30" t="n">
-        <v>1.3595</v>
+        <v>0.5426</v>
       </c>
       <c r="H60" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I60" s="30" t="n">
-        <v>1.3566</v>
+        <v>0.5413</v>
       </c>
       <c r="J60" s="33" t="n">
-        <v>-0.0021</v>
+        <v>-0.0024</v>
       </c>
       <c r="K60" s="8" t="n">
-        <v>-15.45</v>
+        <v>-17.43</v>
       </c>
       <c r="L60" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M60" s="32" t="inlineStr">
         <is>
-          <t>债券</t>
+          <t>A 股</t>
         </is>
       </c>
       <c r="N60" s="32" t="inlineStr">
         <is>
-          <t>国内债券</t>
+          <t>行业股</t>
         </is>
       </c>
       <c r="O60" s="32" t="inlineStr">
         <is>
-          <t>可转债</t>
+          <t>中证环保</t>
         </is>
       </c>
       <c r="P60" s="32" t="inlineStr">
         <is>
-          <t>411</t>
+          <t>143</t>
         </is>
       </c>
       <c r="Q60" s="32" t="inlineStr">
@@ -4626,64 +4626,64 @@
     <row r="61">
       <c r="A61" s="28" t="inlineStr">
         <is>
-          <t>广发中证环保ETF联接A</t>
+          <t>长信可转债债券A</t>
         </is>
       </c>
       <c r="B61" s="29" t="n">
-        <v>1064</v>
+        <v>519977</v>
       </c>
       <c r="C61" s="30" t="n">
-        <v>0.4775</v>
+        <v>1.2011</v>
       </c>
       <c r="D61" s="31" t="n">
-        <v>13403.92</v>
+        <v>5328.62</v>
       </c>
       <c r="E61" s="31" t="n">
-        <v>7219.35</v>
+        <v>7229.87</v>
       </c>
       <c r="F61" s="31" t="n">
-        <v>819.35</v>
+        <v>829.87</v>
       </c>
       <c r="G61" s="30" t="n">
-        <v>0.5389</v>
+        <v>1.3568</v>
       </c>
       <c r="H61" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I61" s="30" t="n">
-        <v>0.5386</v>
+        <v>1.355</v>
       </c>
       <c r="J61" s="33" t="n">
-        <v>-0.0005999999999999999</v>
+        <v>-0.0014</v>
       </c>
       <c r="K61" s="8" t="n">
-        <v>-4.02</v>
+        <v>-9.59</v>
       </c>
       <c r="L61" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M61" s="32" t="inlineStr">
         <is>
-          <t>A 股</t>
+          <t>债券</t>
         </is>
       </c>
       <c r="N61" s="32" t="inlineStr">
         <is>
-          <t>行业股</t>
+          <t>国内债券</t>
         </is>
       </c>
       <c r="O61" s="32" t="inlineStr">
         <is>
-          <t>中证环保</t>
+          <t>可转债</t>
         </is>
       </c>
       <c r="P61" s="32" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>411</t>
         </is>
       </c>
       <c r="Q61" s="32" t="inlineStr">
@@ -4708,31 +4708,31 @@
         <v>7778.64</v>
       </c>
       <c r="E62" s="31" t="n">
-        <v>6700.52</v>
+        <v>6679.51</v>
       </c>
       <c r="F62" s="31" t="n">
-        <v>-299.48</v>
+        <v>-320.49</v>
       </c>
       <c r="G62" s="30" t="n">
-        <v>0.8683999999999999</v>
+        <v>0.8587</v>
       </c>
       <c r="H62" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I62" s="30" t="n">
-        <v>0.8615</v>
+        <v>0.8565</v>
       </c>
       <c r="J62" s="33" t="n">
-        <v>-0.008</v>
+        <v>-0.0026</v>
       </c>
       <c r="K62" s="8" t="n">
-        <v>-53.67</v>
+        <v>-17.11</v>
       </c>
       <c r="L62" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M62" s="32" t="inlineStr">
@@ -4777,31 +4777,31 @@
         <v>7852.99</v>
       </c>
       <c r="E63" s="31" t="n">
-        <v>6002.04</v>
+        <v>5876.39</v>
       </c>
       <c r="F63" s="31" t="n">
-        <v>-397.96</v>
+        <v>-523.61</v>
       </c>
       <c r="G63" s="30" t="n">
-        <v>0.772</v>
+        <v>0.7483</v>
       </c>
       <c r="H63" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I63" s="30" t="n">
-        <v>0.7643</v>
+        <v>0.7485000000000001</v>
       </c>
       <c r="J63" s="33" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="K63" s="8" t="n">
-        <v>-60.47</v>
+        <v>0.0003</v>
+      </c>
+      <c r="K63" s="9" t="n">
+        <v>1.57</v>
       </c>
       <c r="L63" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M63" s="32" t="inlineStr">
@@ -4846,31 +4846,31 @@
         <v>3580.2</v>
       </c>
       <c r="E64" s="31" t="n">
-        <v>3327.79</v>
+        <v>3310.25</v>
       </c>
       <c r="F64" s="31" t="n">
-        <v>-172.21</v>
+        <v>-189.75</v>
       </c>
       <c r="G64" s="30" t="n">
-        <v>0.9407</v>
+        <v>0.9246</v>
       </c>
       <c r="H64" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I64" s="30" t="n">
-        <v>0.9288999999999999</v>
+        <v>0.9199000000000001</v>
       </c>
       <c r="J64" s="33" t="n">
-        <v>-0.0125</v>
+        <v>-0.005</v>
       </c>
       <c r="K64" s="8" t="n">
-        <v>-42.25</v>
+        <v>-16.83</v>
       </c>
       <c r="L64" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M64" s="32" t="inlineStr">
@@ -4909,37 +4909,37 @@
         <v>519671</v>
       </c>
       <c r="C65" s="4" t="n">
-        <v>1.4259</v>
+        <v>1.4262</v>
       </c>
       <c r="D65" s="5" t="n">
-        <v>997.72</v>
+        <v>1013.26</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>1417.76</v>
+        <v>1448.96</v>
       </c>
       <c r="F65" s="5" t="n">
-        <v>-4.89</v>
+        <v>3.86</v>
       </c>
       <c r="G65" s="4" t="n">
-        <v>1.425</v>
+        <v>1.43</v>
       </c>
       <c r="H65" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I65" s="4" t="n">
-        <v>1.4212</v>
+        <v>1.4235</v>
       </c>
       <c r="J65" s="7" t="n">
-        <v>-0.0027</v>
+        <v>-0.0046</v>
       </c>
       <c r="K65" s="8" t="n">
-        <v>-3.79</v>
+        <v>-6.59</v>
       </c>
       <c r="L65" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M65" s="6" t="inlineStr">
@@ -4978,37 +4978,37 @@
         <v>90010</v>
       </c>
       <c r="C66" s="4" t="n">
-        <v>1.6533</v>
+        <v>1.6528</v>
       </c>
       <c r="D66" s="5" t="n">
-        <v>845.95</v>
+        <v>859.89</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>1356.9</v>
+        <v>1382.7</v>
       </c>
       <c r="F66" s="5" t="n">
-        <v>-41.7</v>
+        <v>-38.53</v>
       </c>
       <c r="G66" s="4" t="n">
-        <v>1.61</v>
+        <v>1.608</v>
       </c>
       <c r="H66" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I66" s="4" t="n">
-        <v>1.6043</v>
+        <v>1.6048</v>
       </c>
       <c r="J66" s="7" t="n">
-        <v>-0.0035</v>
+        <v>-0.002</v>
       </c>
       <c r="K66" s="8" t="n">
-        <v>-4.82</v>
+        <v>-2.75</v>
       </c>
       <c r="L66" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M66" s="6" t="inlineStr">
@@ -5053,31 +5053,31 @@
         <v>898.04</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>1299.1</v>
+        <v>1311.86</v>
       </c>
       <c r="F67" s="5" t="n">
-        <v>88.13</v>
+        <v>100.89</v>
       </c>
       <c r="G67" s="4" t="n">
-        <v>1.4466</v>
+        <v>1.4608</v>
       </c>
       <c r="H67" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I67" s="4" t="n">
-        <v>1.4532</v>
+        <v>1.4338</v>
       </c>
       <c r="J67" s="7" t="n">
-        <v>0.0045</v>
-      </c>
-      <c r="K67" s="9" t="n">
-        <v>5.93</v>
+        <v>-0.0185</v>
+      </c>
+      <c r="K67" s="8" t="n">
+        <v>-24.25</v>
       </c>
       <c r="L67" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 16:00</t>
+          <t>2019-11-29 12:00</t>
         </is>
       </c>
       <c r="M67" s="6" t="inlineStr">
@@ -5116,37 +5116,37 @@
         <v>3318</v>
       </c>
       <c r="C68" s="4" t="n">
-        <v>0.9335</v>
+        <v>0.9331</v>
       </c>
       <c r="D68" s="5" t="n">
-        <v>1288.86</v>
+        <v>1312.53</v>
       </c>
       <c r="E68" s="5" t="n">
-        <v>1175.96</v>
+        <v>1193.22</v>
       </c>
       <c r="F68" s="5" t="n">
-        <v>-27.18</v>
+        <v>-31.49</v>
       </c>
       <c r="G68" s="4" t="n">
-        <v>0.9183</v>
+        <v>0.9091</v>
       </c>
       <c r="H68" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I68" s="4" t="n">
-        <v>0.9124</v>
+        <v>0.9094</v>
       </c>
       <c r="J68" s="7" t="n">
-        <v>-0.0065</v>
-      </c>
-      <c r="K68" s="8" t="n">
-        <v>-7.6</v>
+        <v>0.0004</v>
+      </c>
+      <c r="K68" s="9" t="n">
+        <v>0.39</v>
       </c>
       <c r="L68" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M68" s="6" t="inlineStr">
@@ -5185,37 +5185,37 @@
         <v>70023</v>
       </c>
       <c r="C69" s="4" t="n">
-        <v>1.794</v>
+        <v>1.7954</v>
       </c>
       <c r="D69" s="5" t="n">
-        <v>473.31</v>
+        <v>482.9</v>
       </c>
       <c r="E69" s="5" t="n">
-        <v>863.7</v>
+        <v>888.54</v>
       </c>
       <c r="F69" s="5" t="n">
-        <v>14.56</v>
+        <v>21.55</v>
       </c>
       <c r="G69" s="4" t="n">
-        <v>1.8422</v>
+        <v>1.84</v>
       </c>
       <c r="H69" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I69" s="4" t="n">
-        <v>1.8247</v>
+        <v>1.8302</v>
       </c>
       <c r="J69" s="7" t="n">
-        <v>-0.0095</v>
+        <v>-0.0053</v>
       </c>
       <c r="K69" s="8" t="n">
-        <v>-8.279999999999999</v>
+        <v>-4.73</v>
       </c>
       <c r="L69" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M69" s="6" t="inlineStr">
@@ -5254,37 +5254,37 @@
         <v>530015</v>
       </c>
       <c r="C70" s="4" t="n">
-        <v>2.1188</v>
+        <v>2.1198</v>
       </c>
       <c r="D70" s="5" t="n">
-        <v>381.21</v>
+        <v>389.84</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>808.47</v>
+        <v>833.67</v>
       </c>
       <c r="F70" s="5" t="n">
-        <v>0.78</v>
+        <v>7.27</v>
       </c>
       <c r="G70" s="4" t="n">
-        <v>2.1379</v>
+        <v>2.1385</v>
       </c>
       <c r="H70" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I70" s="4" t="n">
-        <v>2.1202</v>
+        <v>2.1279</v>
       </c>
       <c r="J70" s="7" t="n">
-        <v>-0.0083</v>
+        <v>-0.0049</v>
       </c>
       <c r="K70" s="8" t="n">
-        <v>-6.75</v>
+        <v>-4.13</v>
       </c>
       <c r="L70" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M70" s="6" t="inlineStr">
@@ -5323,37 +5323,37 @@
         <v>968</v>
       </c>
       <c r="C71" s="4" t="n">
-        <v>0.961</v>
+        <v>0.9608</v>
       </c>
       <c r="D71" s="5" t="n">
-        <v>336.9</v>
+        <v>354.88</v>
       </c>
       <c r="E71" s="5" t="n">
-        <v>322.01</v>
+        <v>336.04</v>
       </c>
       <c r="F71" s="5" t="n">
-        <v>-1.75</v>
+        <v>-4.94</v>
       </c>
       <c r="G71" s="4" t="n">
-        <v>0.9702</v>
+        <v>0.9469</v>
       </c>
       <c r="H71" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I71" s="4" t="n">
-        <v>0.9556</v>
+        <v>0.9376</v>
       </c>
       <c r="J71" s="7" t="n">
-        <v>-0.015</v>
+        <v>-0.0098</v>
       </c>
       <c r="K71" s="8" t="n">
-        <v>-4.92</v>
+        <v>-3.3</v>
       </c>
       <c r="L71" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M71" s="6" t="inlineStr">
@@ -5398,31 +5398,31 @@
         <v>214.89</v>
       </c>
       <c r="E72" s="5" t="n">
-        <v>200.08</v>
+        <v>200.41</v>
       </c>
       <c r="F72" s="5" t="n">
-        <v>-11.14</v>
+        <v>-10.81</v>
       </c>
       <c r="G72" s="4" t="n">
-        <v>0.9334</v>
+        <v>0.9326</v>
       </c>
       <c r="H72" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I72" s="4" t="n">
-        <v>0.9278</v>
+        <v>0.9268999999999999</v>
       </c>
       <c r="J72" s="7" t="n">
-        <v>-0.006</v>
+        <v>-0.0061</v>
       </c>
       <c r="K72" s="8" t="n">
-        <v>-1.2</v>
+        <v>-1.22</v>
       </c>
       <c r="L72" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M72" s="6" t="inlineStr">
@@ -5467,31 +5467,31 @@
         <v>212.74</v>
       </c>
       <c r="E73" s="5" t="n">
-        <v>166.15</v>
+        <v>164.19</v>
       </c>
       <c r="F73" s="5" t="n">
-        <v>23.45</v>
+        <v>21.49</v>
       </c>
       <c r="G73" s="4" t="n">
-        <v>0.8068</v>
+        <v>0.7718</v>
       </c>
       <c r="H73" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I73" s="4" t="n">
-        <v>0.7812</v>
+        <v>0.7577</v>
       </c>
       <c r="J73" s="7" t="n">
-        <v>-0.0317</v>
+        <v>-0.0182</v>
       </c>
       <c r="K73" s="8" t="n">
-        <v>-5.45</v>
+        <v>-3</v>
       </c>
       <c r="L73" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M73" s="6" t="inlineStr">
@@ -5536,31 +5536,31 @@
         <v>62.09</v>
       </c>
       <c r="E74" s="5" t="n">
-        <v>81.59</v>
+        <v>81.77</v>
       </c>
       <c r="F74" s="5" t="n">
-        <v>1.55</v>
+        <v>1.73</v>
       </c>
       <c r="G74" s="4" t="n">
-        <v>1.32</v>
+        <v>1.317</v>
       </c>
       <c r="H74" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I74" s="4" t="n">
-        <v>1.311</v>
+        <v>1.2915</v>
       </c>
       <c r="J74" s="7" t="n">
-        <v>-0.0068</v>
+        <v>-0.0194</v>
       </c>
       <c r="K74" s="8" t="n">
-        <v>-0.5600000000000001</v>
+        <v>-1.58</v>
       </c>
       <c r="L74" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M74" s="6" t="inlineStr">
@@ -5605,31 +5605,31 @@
         <v>24.24</v>
       </c>
       <c r="E75" s="5" t="n">
-        <v>34.72</v>
+        <v>34.91</v>
       </c>
       <c r="F75" s="5" t="n">
-        <v>-2.36</v>
+        <v>-2.17</v>
       </c>
       <c r="G75" s="4" t="n">
-        <v>1.4361</v>
+        <v>1.44</v>
       </c>
       <c r="H75" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I75" s="4" t="n">
-        <v>1.4323</v>
+        <v>1.4334</v>
       </c>
       <c r="J75" s="7" t="n">
-        <v>-0.0027</v>
+        <v>-0.0046</v>
       </c>
       <c r="K75" s="8" t="n">
-        <v>-0.09</v>
+        <v>-0.16</v>
       </c>
       <c r="L75" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M75" s="6" t="inlineStr">
@@ -5668,37 +5668,37 @@
         <v>90010</v>
       </c>
       <c r="C76" s="4" t="n">
-        <v>1.6593</v>
+        <v>1.6581</v>
       </c>
       <c r="D76" s="5" t="n">
-        <v>890.02</v>
+        <v>917.91</v>
       </c>
       <c r="E76" s="5" t="n">
-        <v>1427.59</v>
+        <v>1476</v>
       </c>
       <c r="F76" s="5" t="n">
-        <v>-49.18</v>
+        <v>-46.03</v>
       </c>
       <c r="G76" s="4" t="n">
-        <v>1.61</v>
+        <v>1.608</v>
       </c>
       <c r="H76" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I76" s="4" t="n">
-        <v>1.6043</v>
+        <v>1.6048</v>
       </c>
       <c r="J76" s="7" t="n">
-        <v>-0.0035</v>
+        <v>-0.002</v>
       </c>
       <c r="K76" s="8" t="n">
-        <v>-5.07</v>
+        <v>-2.94</v>
       </c>
       <c r="L76" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M76" s="6" t="inlineStr">
@@ -5737,37 +5737,37 @@
         <v>519671</v>
       </c>
       <c r="C77" s="4" t="n">
-        <v>1.4239</v>
+        <v>1.4245</v>
       </c>
       <c r="D77" s="5" t="n">
-        <v>962.45</v>
+        <v>993.53</v>
       </c>
       <c r="E77" s="5" t="n">
-        <v>1367.64</v>
+        <v>1420.75</v>
       </c>
       <c r="F77" s="5" t="n">
-        <v>-2.77</v>
+        <v>5.44</v>
       </c>
       <c r="G77" s="4" t="n">
-        <v>1.425</v>
+        <v>1.43</v>
       </c>
       <c r="H77" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I77" s="4" t="n">
-        <v>1.4212</v>
+        <v>1.4235</v>
       </c>
       <c r="J77" s="7" t="n">
-        <v>-0.0027</v>
+        <v>-0.0046</v>
       </c>
       <c r="K77" s="8" t="n">
-        <v>-3.66</v>
+        <v>-6.46</v>
       </c>
       <c r="L77" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M77" s="6" t="inlineStr">
@@ -5812,31 +5812,31 @@
         <v>915.97</v>
       </c>
       <c r="E78" s="5" t="n">
-        <v>1325.04</v>
+        <v>1338.05</v>
       </c>
       <c r="F78" s="5" t="n">
-        <v>87.2</v>
+        <v>100.21</v>
       </c>
       <c r="G78" s="4" t="n">
-        <v>1.4466</v>
+        <v>1.4608</v>
       </c>
       <c r="H78" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I78" s="4" t="n">
-        <v>1.4532</v>
+        <v>1.4338</v>
       </c>
       <c r="J78" s="7" t="n">
-        <v>0.0045</v>
-      </c>
-      <c r="K78" s="9" t="n">
-        <v>6.05</v>
+        <v>-0.0185</v>
+      </c>
+      <c r="K78" s="8" t="n">
+        <v>-24.73</v>
       </c>
       <c r="L78" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 16:00</t>
+          <t>2019-11-29 12:00</t>
         </is>
       </c>
       <c r="M78" s="6" t="inlineStr">
@@ -5875,37 +5875,37 @@
         <v>3318</v>
       </c>
       <c r="C79" s="4" t="n">
-        <v>0.9348</v>
+        <v>0.9339</v>
       </c>
       <c r="D79" s="5" t="n">
-        <v>1272.96</v>
+        <v>1320.32</v>
       </c>
       <c r="E79" s="5" t="n">
-        <v>1161.45</v>
+        <v>1200.3</v>
       </c>
       <c r="F79" s="5" t="n">
-        <v>-28.52</v>
+        <v>-32.81</v>
       </c>
       <c r="G79" s="4" t="n">
-        <v>0.9183</v>
+        <v>0.9091</v>
       </c>
       <c r="H79" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I79" s="4" t="n">
-        <v>0.9124</v>
+        <v>0.9094</v>
       </c>
       <c r="J79" s="7" t="n">
-        <v>-0.0065</v>
-      </c>
-      <c r="K79" s="8" t="n">
-        <v>-7.51</v>
+        <v>0.0004</v>
+      </c>
+      <c r="K79" s="9" t="n">
+        <v>0.4</v>
       </c>
       <c r="L79" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M79" s="6" t="inlineStr">
@@ -5944,37 +5944,37 @@
         <v>70023</v>
       </c>
       <c r="C80" s="4" t="n">
-        <v>1.7945</v>
+        <v>1.7969</v>
       </c>
       <c r="D80" s="5" t="n">
-        <v>490.43</v>
+        <v>509.62</v>
       </c>
       <c r="E80" s="5" t="n">
-        <v>894.9400000000001</v>
+        <v>937.7</v>
       </c>
       <c r="F80" s="5" t="n">
-        <v>14.87</v>
+        <v>21.94</v>
       </c>
       <c r="G80" s="4" t="n">
-        <v>1.8422</v>
+        <v>1.84</v>
       </c>
       <c r="H80" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I80" s="4" t="n">
-        <v>1.8247</v>
+        <v>1.8302</v>
       </c>
       <c r="J80" s="7" t="n">
-        <v>-0.0095</v>
+        <v>-0.0053</v>
       </c>
       <c r="K80" s="8" t="n">
-        <v>-8.58</v>
+        <v>-4.99</v>
       </c>
       <c r="L80" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M80" s="6" t="inlineStr">
@@ -6013,37 +6013,37 @@
         <v>530015</v>
       </c>
       <c r="C81" s="4" t="n">
-        <v>2.1185</v>
+        <v>2.1207</v>
       </c>
       <c r="D81" s="5" t="n">
-        <v>355.38</v>
+        <v>372.65</v>
       </c>
       <c r="E81" s="5" t="n">
-        <v>753.6900000000001</v>
+        <v>796.91</v>
       </c>
       <c r="F81" s="5" t="n">
-        <v>0.83</v>
+        <v>6.62</v>
       </c>
       <c r="G81" s="4" t="n">
-        <v>2.1379</v>
+        <v>2.1385</v>
       </c>
       <c r="H81" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I81" s="4" t="n">
-        <v>2.1202</v>
+        <v>2.1279</v>
       </c>
       <c r="J81" s="7" t="n">
-        <v>-0.0083</v>
+        <v>-0.0049</v>
       </c>
       <c r="K81" s="8" t="n">
-        <v>-6.29</v>
+        <v>-3.95</v>
       </c>
       <c r="L81" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M81" s="6" t="inlineStr">
@@ -6082,37 +6082,37 @@
         <v>968</v>
       </c>
       <c r="C82" s="4" t="n">
-        <v>0.9608</v>
+        <v>0.9605</v>
       </c>
       <c r="D82" s="5" t="n">
-        <v>319.14</v>
+        <v>355.1</v>
       </c>
       <c r="E82" s="5" t="n">
-        <v>305.03</v>
+        <v>336.24</v>
       </c>
       <c r="F82" s="5" t="n">
-        <v>-1.59</v>
+        <v>-4.82</v>
       </c>
       <c r="G82" s="4" t="n">
-        <v>0.9702</v>
+        <v>0.9469</v>
       </c>
       <c r="H82" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I82" s="4" t="n">
-        <v>0.9556</v>
+        <v>0.9376</v>
       </c>
       <c r="J82" s="7" t="n">
-        <v>-0.015</v>
+        <v>-0.0098</v>
       </c>
       <c r="K82" s="8" t="n">
-        <v>-4.66</v>
+        <v>-3.3</v>
       </c>
       <c r="L82" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M82" s="6" t="inlineStr">
@@ -6157,31 +6157,31 @@
         <v>227.52</v>
       </c>
       <c r="E83" s="5" t="n">
-        <v>211.84</v>
+        <v>212.19</v>
       </c>
       <c r="F83" s="5" t="n">
-        <v>-11.67</v>
+        <v>-11.32</v>
       </c>
       <c r="G83" s="4" t="n">
-        <v>0.9334</v>
+        <v>0.9326</v>
       </c>
       <c r="H83" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I83" s="4" t="n">
-        <v>0.9278</v>
+        <v>0.9268999999999999</v>
       </c>
       <c r="J83" s="7" t="n">
-        <v>-0.006</v>
+        <v>-0.0061</v>
       </c>
       <c r="K83" s="8" t="n">
-        <v>-1.27</v>
+        <v>-1.3</v>
       </c>
       <c r="L83" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M83" s="6" t="inlineStr">
@@ -6226,31 +6226,31 @@
         <v>142.1</v>
       </c>
       <c r="E84" s="5" t="n">
-        <v>186.72</v>
+        <v>187.15</v>
       </c>
       <c r="F84" s="5" t="n">
-        <v>4.27</v>
+        <v>4.7</v>
       </c>
       <c r="G84" s="4" t="n">
-        <v>1.32</v>
+        <v>1.317</v>
       </c>
       <c r="H84" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I84" s="4" t="n">
-        <v>1.311</v>
+        <v>1.2915</v>
       </c>
       <c r="J84" s="7" t="n">
-        <v>-0.0068</v>
+        <v>-0.0194</v>
       </c>
       <c r="K84" s="8" t="n">
-        <v>-1.28</v>
+        <v>-3.62</v>
       </c>
       <c r="L84" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M84" s="6" t="inlineStr">
@@ -6295,31 +6295,31 @@
         <v>212.74</v>
       </c>
       <c r="E85" s="5" t="n">
-        <v>166.15</v>
+        <v>164.19</v>
       </c>
       <c r="F85" s="5" t="n">
-        <v>23.45</v>
+        <v>21.49</v>
       </c>
       <c r="G85" s="4" t="n">
-        <v>0.8068</v>
+        <v>0.7718</v>
       </c>
       <c r="H85" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I85" s="4" t="n">
-        <v>0.7812</v>
+        <v>0.7577</v>
       </c>
       <c r="J85" s="7" t="n">
-        <v>-0.0317</v>
+        <v>-0.0182</v>
       </c>
       <c r="K85" s="8" t="n">
-        <v>-5.45</v>
+        <v>-3</v>
       </c>
       <c r="L85" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M85" s="6" t="inlineStr">
@@ -6364,31 +6364,31 @@
         <v>24.24</v>
       </c>
       <c r="E86" s="5" t="n">
-        <v>34.72</v>
+        <v>34.91</v>
       </c>
       <c r="F86" s="5" t="n">
-        <v>-2.36</v>
+        <v>-2.17</v>
       </c>
       <c r="G86" s="4" t="n">
-        <v>1.4361</v>
+        <v>1.44</v>
       </c>
       <c r="H86" s="6" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I86" s="4" t="n">
-        <v>1.4323</v>
+        <v>1.4334</v>
       </c>
       <c r="J86" s="7" t="n">
-        <v>-0.0027</v>
+        <v>-0.0046</v>
       </c>
       <c r="K86" s="8" t="n">
-        <v>-0.09</v>
+        <v>-0.16</v>
       </c>
       <c r="L86" s="6" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M86" s="6" t="inlineStr">
@@ -6427,37 +6427,37 @@
         <v>162711</v>
       </c>
       <c r="C87" s="30" t="n">
-        <v>1.0519</v>
+        <v>0</v>
       </c>
       <c r="D87" s="31" t="n">
-        <v>9697.57</v>
+        <v>0</v>
       </c>
       <c r="E87" s="31" t="n">
-        <v>10454.95</v>
+        <v>10421.97</v>
       </c>
       <c r="F87" s="31" t="n">
-        <v>254.95</v>
+        <v>221.97</v>
       </c>
       <c r="G87" s="30" t="n">
-        <v>1.0869</v>
+        <v>1.0747</v>
       </c>
       <c r="H87" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I87" s="30" t="n">
-        <v>1.0782</v>
+        <v>1.0719</v>
       </c>
       <c r="J87" s="33" t="n">
-        <v>-0.008</v>
-      </c>
-      <c r="K87" s="8" t="n">
-        <v>-84.37</v>
+        <v>-0.0026</v>
+      </c>
+      <c r="K87" s="9" t="n">
+        <v>-0</v>
       </c>
       <c r="L87" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M87" s="32" t="inlineStr">
@@ -6496,37 +6496,37 @@
         <v>100032</v>
       </c>
       <c r="C88" s="30" t="n">
-        <v>1.0142</v>
+        <v>1.0193</v>
       </c>
       <c r="D88" s="31" t="n">
-        <v>8677.6</v>
+        <v>65064.33</v>
       </c>
       <c r="E88" s="31" t="n">
-        <v>9449.9</v>
+        <v>9475.93</v>
       </c>
       <c r="F88" s="31" t="n">
-        <v>649.9</v>
+        <v>675.9299999999999</v>
       </c>
       <c r="G88" s="30" t="n">
-        <v>1.095</v>
+        <v>1.092</v>
       </c>
       <c r="H88" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I88" s="30" t="n">
-        <v>1.0912</v>
+        <v>1.0898</v>
       </c>
       <c r="J88" s="33" t="n">
-        <v>-0.0035</v>
+        <v>-0.002</v>
       </c>
       <c r="K88" s="8" t="n">
-        <v>-32.97</v>
+        <v>-143.14</v>
       </c>
       <c r="L88" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M88" s="32" t="inlineStr">
@@ -6565,37 +6565,37 @@
         <v>968</v>
       </c>
       <c r="C89" s="30" t="n">
-        <v>0.853</v>
+        <v>0.9167</v>
       </c>
       <c r="D89" s="31" t="n">
-        <v>6096.21</v>
+        <v>63490</v>
       </c>
       <c r="E89" s="31" t="n">
-        <v>5826.75</v>
+        <v>5772.5</v>
       </c>
       <c r="F89" s="31" t="n">
-        <v>626.75</v>
+        <v>572.5</v>
       </c>
       <c r="G89" s="30" t="n">
-        <v>0.9702</v>
+        <v>0.9469</v>
       </c>
       <c r="H89" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I89" s="30" t="n">
-        <v>0.9556</v>
+        <v>0.9376</v>
       </c>
       <c r="J89" s="33" t="n">
-        <v>-0.015</v>
+        <v>-0.0098</v>
       </c>
       <c r="K89" s="8" t="n">
-        <v>-89</v>
+        <v>-590.46</v>
       </c>
       <c r="L89" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M89" s="32" t="inlineStr">
@@ -6634,37 +6634,37 @@
         <v>1180</v>
       </c>
       <c r="C90" s="30" t="n">
-        <v>0.7111</v>
+        <v>0.7451</v>
       </c>
       <c r="D90" s="31" t="n">
-        <v>6750.28</v>
+        <v>41014.88</v>
       </c>
       <c r="E90" s="31" t="n">
-        <v>5768.78</v>
+        <v>5720.86</v>
       </c>
       <c r="F90" s="31" t="n">
-        <v>968.78</v>
+        <v>920.86</v>
       </c>
       <c r="G90" s="30" t="n">
-        <v>0.8803</v>
+        <v>0.8475</v>
       </c>
       <c r="H90" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I90" s="30" t="n">
-        <v>0.8542999999999999</v>
+        <v>0.8276</v>
       </c>
       <c r="J90" s="33" t="n">
-        <v>-0.0295</v>
+        <v>-0.0235</v>
       </c>
       <c r="K90" s="8" t="n">
-        <v>-175.51</v>
+        <v>-816.2</v>
       </c>
       <c r="L90" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M90" s="32" t="inlineStr">
@@ -6703,37 +6703,37 @@
         <v>100038</v>
       </c>
       <c r="C91" s="30" t="n">
-        <v>1.3043</v>
+        <v>1.3129</v>
       </c>
       <c r="D91" s="31" t="n">
-        <v>2760.12</v>
+        <v>14624.61</v>
       </c>
       <c r="E91" s="31" t="n">
-        <v>4435.51</v>
+        <v>4441.03</v>
       </c>
       <c r="F91" s="31" t="n">
-        <v>835.51</v>
+        <v>841.03</v>
       </c>
       <c r="G91" s="30" t="n">
-        <v>1.626</v>
+        <v>1.609</v>
       </c>
       <c r="H91" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I91" s="30" t="n">
-        <v>1.6102</v>
+        <v>1.5936</v>
       </c>
       <c r="J91" s="33" t="n">
-        <v>-0.0097</v>
+        <v>-0.009599999999999999</v>
       </c>
       <c r="K91" s="8" t="n">
-        <v>-43.61</v>
+        <v>-225.22</v>
       </c>
       <c r="L91" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M91" s="32" t="inlineStr">
@@ -6772,37 +6772,37 @@
         <v>4752</v>
       </c>
       <c r="C92" s="30" t="n">
-        <v>0.7235</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="D92" s="31" t="n">
-        <v>4423.48</v>
+        <v>7852.99</v>
       </c>
       <c r="E92" s="31" t="n">
-        <v>3380.86</v>
+        <v>3310.09</v>
       </c>
       <c r="F92" s="31" t="n">
-        <v>180.86</v>
+        <v>110.09</v>
       </c>
       <c r="G92" s="30" t="n">
-        <v>0.772</v>
+        <v>0.7483</v>
       </c>
       <c r="H92" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I92" s="30" t="n">
-        <v>0.7643</v>
+        <v>0.7485000000000001</v>
       </c>
       <c r="J92" s="33" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="K92" s="8" t="n">
-        <v>-34.06</v>
+        <v>0.0003</v>
+      </c>
+      <c r="K92" s="9" t="n">
+        <v>1.57</v>
       </c>
       <c r="L92" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M92" s="32" t="inlineStr">
@@ -6841,37 +6841,37 @@
         <v>161017</v>
       </c>
       <c r="C93" s="30" t="n">
-        <v>1.325</v>
+        <v>1.3432</v>
       </c>
       <c r="D93" s="31" t="n">
-        <v>2046.97</v>
+        <v>9529.809999999999</v>
       </c>
       <c r="E93" s="31" t="n">
-        <v>3250.58</v>
+        <v>3246.49</v>
       </c>
       <c r="F93" s="31" t="n">
-        <v>538.47</v>
+        <v>534.38</v>
       </c>
       <c r="G93" s="30" t="n">
-        <v>1.605</v>
+        <v>1.586</v>
       </c>
       <c r="H93" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I93" s="30" t="n">
-        <v>1.5922</v>
+        <v>1.5819</v>
       </c>
       <c r="J93" s="33" t="n">
-        <v>-0.008</v>
+        <v>-0.0026</v>
       </c>
       <c r="K93" s="8" t="n">
-        <v>-26.2</v>
+        <v>-39.07</v>
       </c>
       <c r="L93" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M93" s="32" t="inlineStr">
@@ -6910,37 +6910,37 @@
         <v>1064</v>
       </c>
       <c r="C94" s="30" t="n">
-        <v>0.5379</v>
+        <v>0.4775</v>
       </c>
       <c r="D94" s="31" t="n">
-        <v>5949.77</v>
+        <v>13403.92</v>
       </c>
       <c r="E94" s="31" t="n">
-        <v>3204.54</v>
+        <v>3228.34</v>
       </c>
       <c r="F94" s="31" t="n">
-        <v>4.54</v>
+        <v>28.34</v>
       </c>
       <c r="G94" s="30" t="n">
-        <v>0.5389</v>
+        <v>0.5426</v>
       </c>
       <c r="H94" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I94" s="30" t="n">
-        <v>0.5386</v>
+        <v>0.5413</v>
       </c>
       <c r="J94" s="33" t="n">
-        <v>-0.0005999999999999999</v>
+        <v>-0.0024</v>
       </c>
       <c r="K94" s="8" t="n">
-        <v>-1.78</v>
+        <v>-17.43</v>
       </c>
       <c r="L94" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M94" s="32" t="inlineStr">
@@ -6979,10 +6979,10 @@
         <v>110027</v>
       </c>
       <c r="C95" s="30" t="n">
-        <v>1.6007</v>
+        <v>1.5931</v>
       </c>
       <c r="D95" s="31" t="n">
-        <v>1743.65</v>
+        <v>20086.63</v>
       </c>
       <c r="E95" s="31" t="n">
         <v>2931.07</v>
@@ -6991,25 +6991,25 @@
         <v>140.07</v>
       </c>
       <c r="G95" s="30" t="n">
-        <v>1.688</v>
+        <v>1.681</v>
       </c>
       <c r="H95" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I95" s="30" t="n">
-        <v>1.6841</v>
+        <v>1.678</v>
       </c>
       <c r="J95" s="33" t="n">
-        <v>-0.0023</v>
+        <v>-0.0018</v>
       </c>
       <c r="K95" s="8" t="n">
-        <v>-6.8</v>
+        <v>-60.26</v>
       </c>
       <c r="L95" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M95" s="32" t="inlineStr">
@@ -7048,16 +7048,16 @@
         <v>614</v>
       </c>
       <c r="C96" s="30" t="n">
-        <v>1.0612</v>
+        <v>1.091</v>
       </c>
       <c r="D96" s="31" t="n">
-        <v>1884.74</v>
+        <v>20716.63</v>
       </c>
       <c r="E96" s="31" t="n">
-        <v>2263.57</v>
+        <v>2278.65</v>
       </c>
       <c r="F96" s="31" t="n">
-        <v>263.57</v>
+        <v>278.65</v>
       </c>
       <c r="G96" s="30" t="n">
         <v>0</v>
@@ -7117,37 +7117,37 @@
         <v>110026</v>
       </c>
       <c r="C97" s="30" t="n">
-        <v>1.319</v>
+        <v>1.3359</v>
       </c>
       <c r="D97" s="31" t="n">
-        <v>1213.09</v>
+        <v>4791.13</v>
       </c>
       <c r="E97" s="31" t="n">
-        <v>2110.41</v>
+        <v>2103.37</v>
       </c>
       <c r="F97" s="31" t="n">
-        <v>510.41</v>
+        <v>503.37</v>
       </c>
       <c r="G97" s="30" t="n">
-        <v>1.7723</v>
+        <v>1.7339</v>
       </c>
       <c r="H97" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I97" s="30" t="n">
-        <v>1.7395</v>
+        <v>1.7174</v>
       </c>
       <c r="J97" s="33" t="n">
-        <v>-0.0185</v>
+        <v>-0.0095</v>
       </c>
       <c r="K97" s="8" t="n">
-        <v>-39.79</v>
+        <v>-79.05</v>
       </c>
       <c r="L97" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M97" s="32" t="inlineStr">
@@ -7186,37 +7186,37 @@
         <v>340001</v>
       </c>
       <c r="C98" s="30" t="n">
-        <v>0.9816</v>
+        <v>0.9886</v>
       </c>
       <c r="D98" s="31" t="n">
-        <v>1630.08</v>
+        <v>32370.29</v>
       </c>
       <c r="E98" s="31" t="n">
-        <v>1865.95</v>
+        <v>1867.25</v>
       </c>
       <c r="F98" s="31" t="n">
-        <v>265.95</v>
+        <v>267.25</v>
       </c>
       <c r="G98" s="30" t="n">
-        <v>1.1484</v>
+        <v>1.1455</v>
       </c>
       <c r="H98" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I98" s="30" t="n">
-        <v>1.1459</v>
+        <v>1.1442</v>
       </c>
       <c r="J98" s="33" t="n">
-        <v>-0.0022</v>
+        <v>-0.0012</v>
       </c>
       <c r="K98" s="8" t="n">
-        <v>-4.08</v>
+        <v>-42.08</v>
       </c>
       <c r="L98" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M98" s="32" t="inlineStr">
@@ -7255,37 +7255,37 @@
         <v>164906</v>
       </c>
       <c r="C99" s="30" t="n">
-        <v>1.137</v>
+        <v>1.1444</v>
       </c>
       <c r="D99" s="31" t="n">
-        <v>1407.29</v>
+        <v>16778.47</v>
       </c>
       <c r="E99" s="31" t="n">
-        <v>1752.07</v>
+        <v>1851.99</v>
       </c>
       <c r="F99" s="31" t="n">
-        <v>152.07</v>
+        <v>251.99</v>
       </c>
       <c r="G99" s="30" t="n">
-        <v>1.245</v>
+        <v>1.316</v>
       </c>
       <c r="H99" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="I99" s="30" t="n">
-        <v>1.2482</v>
+        <v>1.3174</v>
       </c>
       <c r="J99" s="33" t="n">
-        <v>0.0026</v>
+        <v>0.0011</v>
       </c>
       <c r="K99" s="9" t="n">
-        <v>4.5</v>
+        <v>23.49</v>
       </c>
       <c r="L99" s="32" t="inlineStr">
         <is>
-          <t>2019-11-23 05:00</t>
+          <t>2019-11-28 05:00</t>
         </is>
       </c>
       <c r="M99" s="32" t="inlineStr">
@@ -7324,37 +7324,37 @@
         <v>1051</v>
       </c>
       <c r="C100" s="30" t="n">
-        <v>0.8966</v>
+        <v>0</v>
       </c>
       <c r="D100" s="31" t="n">
-        <v>1338.46</v>
+        <v>0</v>
       </c>
       <c r="E100" s="31" t="n">
-        <v>1339.79</v>
+        <v>1343.81</v>
       </c>
       <c r="F100" s="31" t="n">
-        <v>139.79</v>
+        <v>143.81</v>
       </c>
       <c r="G100" s="30" t="n">
-        <v>1.01</v>
+        <v>1.004</v>
       </c>
       <c r="H100" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I100" s="30" t="n">
-        <v>1.0012</v>
+        <v>0.9925</v>
       </c>
       <c r="J100" s="33" t="n">
-        <v>-0.008699999999999999</v>
-      </c>
-      <c r="K100" s="8" t="n">
-        <v>-11.78</v>
+        <v>-0.0115</v>
+      </c>
+      <c r="K100" s="9" t="n">
+        <v>-0</v>
       </c>
       <c r="L100" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M100" s="32" t="inlineStr">
@@ -7393,37 +7393,37 @@
         <v>162411</v>
       </c>
       <c r="C101" s="30" t="n">
-        <v>0.4776</v>
+        <v>0.5152</v>
       </c>
       <c r="D101" s="31" t="n">
-        <v>3350.7</v>
+        <v>37267.45</v>
       </c>
       <c r="E101" s="31" t="n">
-        <v>1253.16</v>
+        <v>1249.81</v>
       </c>
       <c r="F101" s="31" t="n">
-        <v>-346.84</v>
+        <v>-350.19</v>
       </c>
       <c r="G101" s="30" t="n">
-        <v>0.374</v>
+        <v>0.373</v>
       </c>
       <c r="H101" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="I101" s="30" t="n">
-        <v>0.3753</v>
+        <v>0.3735</v>
       </c>
       <c r="J101" s="33" t="n">
-        <v>0.0035</v>
+        <v>0.0014</v>
       </c>
       <c r="K101" s="9" t="n">
-        <v>4.36</v>
+        <v>18.63</v>
       </c>
       <c r="L101" s="32" t="inlineStr">
         <is>
-          <t>2019-11-23 05:00</t>
+          <t>2019-11-28 05:00</t>
         </is>
       </c>
       <c r="M101" s="32" t="inlineStr">
@@ -7462,37 +7462,37 @@
         <v>162413</v>
       </c>
       <c r="C102" s="30" t="n">
-        <v>0.8027</v>
+        <v>0</v>
       </c>
       <c r="D102" s="31" t="n">
-        <v>1495.03</v>
+        <v>0</v>
       </c>
       <c r="E102" s="31" t="n">
-        <v>1190.19</v>
+        <v>1180.02</v>
       </c>
       <c r="F102" s="31" t="n">
-        <v>-9.81</v>
+        <v>-19.98</v>
       </c>
       <c r="G102" s="30" t="n">
-        <v>0.8058999999999999</v>
+        <v>0.7893</v>
       </c>
       <c r="H102" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I102" s="30" t="n">
-        <v>0.7958</v>
+        <v>0.7853</v>
       </c>
       <c r="J102" s="33" t="n">
-        <v>-0.0125</v>
-      </c>
-      <c r="K102" s="8" t="n">
-        <v>-15.1</v>
+        <v>-0.005</v>
+      </c>
+      <c r="K102" s="9" t="n">
+        <v>-0</v>
       </c>
       <c r="L102" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M102" s="32" t="inlineStr">
@@ -7531,37 +7531,37 @@
         <v>1469</v>
       </c>
       <c r="C103" s="30" t="n">
-        <v>0.8885999999999999</v>
+        <v>0.9073</v>
       </c>
       <c r="D103" s="31" t="n">
-        <v>900.35</v>
+        <v>21163.93</v>
       </c>
       <c r="E103" s="31" t="n">
-        <v>970.39</v>
+        <v>971.65</v>
       </c>
       <c r="F103" s="31" t="n">
-        <v>170.39</v>
+        <v>171.65</v>
       </c>
       <c r="G103" s="30" t="n">
-        <v>1.0826</v>
+        <v>1.0792</v>
       </c>
       <c r="H103" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I103" s="30" t="n">
-        <v>1.0777</v>
+        <v>1.0764</v>
       </c>
       <c r="J103" s="33" t="n">
-        <v>-0.0046</v>
+        <v>-0.0026</v>
       </c>
       <c r="K103" s="8" t="n">
-        <v>-4.41</v>
+        <v>-59.26</v>
       </c>
       <c r="L103" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M103" s="32" t="inlineStr">
@@ -7600,37 +7600,37 @@
         <v>216</v>
       </c>
       <c r="C104" s="30" t="n">
-        <v>1.0903</v>
+        <v>0</v>
       </c>
       <c r="D104" s="31" t="n">
-        <v>733.79</v>
+        <v>0</v>
       </c>
       <c r="E104" s="31" t="n">
-        <v>896.17</v>
+        <v>887.37</v>
       </c>
       <c r="F104" s="31" t="n">
-        <v>96.17</v>
+        <v>87.37</v>
       </c>
       <c r="G104" s="30" t="n">
-        <v>1.2202</v>
+        <v>1.2093</v>
       </c>
       <c r="H104" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I104" s="30" t="n">
-        <v>1.2219</v>
+        <v>1.2098</v>
       </c>
       <c r="J104" s="33" t="n">
-        <v>0.0014</v>
+        <v>0.0005</v>
       </c>
       <c r="K104" s="9" t="n">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="L104" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:30</t>
+          <t>2019-11-29 11:35</t>
         </is>
       </c>
       <c r="M104" s="32" t="inlineStr">
@@ -7669,37 +7669,37 @@
         <v>502010</v>
       </c>
       <c r="C105" s="30" t="n">
-        <v>0.8063</v>
+        <v>0</v>
       </c>
       <c r="D105" s="31" t="n">
-        <v>496.13</v>
+        <v>0</v>
       </c>
       <c r="E105" s="31" t="n">
-        <v>478.26</v>
+        <v>476.83</v>
       </c>
       <c r="F105" s="31" t="n">
-        <v>78.26000000000001</v>
+        <v>76.83</v>
       </c>
       <c r="G105" s="30" t="n">
-        <v>0.9671999999999999</v>
+        <v>0.9611</v>
       </c>
       <c r="H105" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I105" s="30" t="n">
-        <v>0.9643</v>
+        <v>0.965</v>
       </c>
       <c r="J105" s="33" t="n">
-        <v>-0.003</v>
-      </c>
-      <c r="K105" s="8" t="n">
-        <v>-1.44</v>
+        <v>0.0041</v>
+      </c>
+      <c r="K105" s="9" t="n">
+        <v>0</v>
       </c>
       <c r="L105" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M105" s="32" t="inlineStr">
@@ -7738,37 +7738,37 @@
         <v>3765</v>
       </c>
       <c r="C106" s="30" t="n">
-        <v>0.8121</v>
+        <v>0</v>
       </c>
       <c r="D106" s="31" t="n">
-        <v>492.57</v>
+        <v>0</v>
       </c>
       <c r="E106" s="31" t="n">
-        <v>465.77</v>
+        <v>463.85</v>
       </c>
       <c r="F106" s="31" t="n">
-        <v>65.77</v>
+        <v>63.85</v>
       </c>
       <c r="G106" s="30" t="n">
-        <v>0.9631</v>
+        <v>0.9417</v>
       </c>
       <c r="H106" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I106" s="30" t="n">
-        <v>0.9453</v>
+        <v>0.9328</v>
       </c>
       <c r="J106" s="33" t="n">
-        <v>-0.0185</v>
-      </c>
-      <c r="K106" s="8" t="n">
-        <v>-8.77</v>
+        <v>-0.0095</v>
+      </c>
+      <c r="K106" s="9" t="n">
+        <v>-0</v>
       </c>
       <c r="L106" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M106" s="32" t="inlineStr">
@@ -7810,34 +7810,34 @@
         <v>1.2011</v>
       </c>
       <c r="D107" s="31" t="n">
-        <v>333.04</v>
+        <v>5328.62</v>
       </c>
       <c r="E107" s="31" t="n">
-        <v>452</v>
+        <v>451.86</v>
       </c>
       <c r="F107" s="31" t="n">
-        <v>52</v>
+        <v>51.86</v>
       </c>
       <c r="G107" s="30" t="n">
-        <v>1.3595</v>
+        <v>1.3568</v>
       </c>
       <c r="H107" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I107" s="30" t="n">
-        <v>1.3566</v>
+        <v>1.355</v>
       </c>
       <c r="J107" s="33" t="n">
-        <v>-0.0021</v>
+        <v>-0.0014</v>
       </c>
       <c r="K107" s="8" t="n">
-        <v>-0.97</v>
+        <v>-9.59</v>
       </c>
       <c r="L107" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M107" s="32" t="inlineStr">
@@ -7876,37 +7876,37 @@
         <v>51</v>
       </c>
       <c r="C108" s="30" t="n">
-        <v>1.2285</v>
+        <v>0</v>
       </c>
       <c r="D108" s="31" t="n">
-        <v>325.61</v>
+        <v>0</v>
       </c>
       <c r="E108" s="31" t="n">
-        <v>420.36</v>
+        <v>421.66</v>
       </c>
       <c r="F108" s="31" t="n">
-        <v>20.36</v>
+        <v>21.66</v>
       </c>
       <c r="G108" s="30" t="n">
-        <v>1.303</v>
+        <v>1.295</v>
       </c>
       <c r="H108" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I108" s="30" t="n">
-        <v>1.2904</v>
+        <v>1.2826</v>
       </c>
       <c r="J108" s="33" t="n">
-        <v>-0.0097</v>
-      </c>
-      <c r="K108" s="8" t="n">
-        <v>-4.1</v>
+        <v>-0.009599999999999999</v>
+      </c>
+      <c r="K108" s="9" t="n">
+        <v>-0</v>
       </c>
       <c r="L108" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M108" s="32" t="inlineStr">
@@ -7945,37 +7945,37 @@
         <v>71</v>
       </c>
       <c r="C109" s="30" t="n">
-        <v>1.452</v>
+        <v>1.4562</v>
       </c>
       <c r="D109" s="31" t="n">
-        <v>275.49</v>
+        <v>6798.52</v>
       </c>
       <c r="E109" s="31" t="n">
-        <v>410.81</v>
+        <v>414.58</v>
       </c>
       <c r="F109" s="31" t="n">
-        <v>10.81</v>
+        <v>14.58</v>
       </c>
       <c r="G109" s="30" t="n">
-        <v>1.4912</v>
+        <v>1.5049</v>
       </c>
       <c r="H109" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I109" s="30" t="n">
-        <v>1.4981</v>
+        <v>1.4767</v>
       </c>
       <c r="J109" s="33" t="n">
-        <v>0.0046</v>
-      </c>
-      <c r="K109" s="9" t="n">
-        <v>1.9</v>
+        <v>-0.0187</v>
+      </c>
+      <c r="K109" s="8" t="n">
+        <v>-191.72</v>
       </c>
       <c r="L109" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 16:00</t>
+          <t>2019-11-29 12:00</t>
         </is>
       </c>
       <c r="M109" s="32" t="inlineStr">
@@ -8014,37 +8014,37 @@
         <v>2903</v>
       </c>
       <c r="C110" s="30" t="n">
-        <v>0.829</v>
+        <v>0.9</v>
       </c>
       <c r="D110" s="31" t="n">
-        <v>275.96</v>
+        <v>7778.64</v>
       </c>
       <c r="E110" s="31" t="n">
-        <v>237.71</v>
+        <v>236.96</v>
       </c>
       <c r="F110" s="31" t="n">
-        <v>8.949999999999999</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="G110" s="30" t="n">
-        <v>0.8683999999999999</v>
+        <v>0.8587</v>
       </c>
       <c r="H110" s="32" t="inlineStr">
         <is>
-          <t>2019-11-21</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="I110" s="30" t="n">
-        <v>0.8615</v>
+        <v>0.8565</v>
       </c>
       <c r="J110" s="33" t="n">
-        <v>-0.008</v>
+        <v>-0.0026</v>
       </c>
       <c r="K110" s="8" t="n">
-        <v>-1.9</v>
+        <v>-17.11</v>
       </c>
       <c r="L110" s="32" t="inlineStr">
         <is>
-          <t>2019-11-22 15:00</t>
+          <t>2019-11-29 11:30</t>
         </is>
       </c>
       <c r="M110" s="32" t="inlineStr">

</xml_diff>